<commit_message>
Latex code documents added
</commit_message>
<xml_diff>
--- a/uomBirds.xlsx
+++ b/uomBirds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF2651F-0DC2-4A81-8FD5-A5497467FCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA10236-1603-4D64-8571-A02998526BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="437">
   <si>
     <t>Common Name</t>
   </si>
@@ -985,9 +985,6 @@
     <t>Loten's sunbirds are compact, measuring only 12–13 cm in length. Their distinguishing feature from the syntopic purple sunbird is their long bill. The wings exhibit a browner hue, and under favorable lighting conditions, the male's maroon breast band becomes visible. Adult males showcase pectoral tufts in a mix of yellow and crimson, utilized in displays. The male's overall plumage is glossy purple with a grey-brown belly. In contrast, females exhibit yellow-grey upperparts and yellowish underparts, lacking the faint supercilium seen in the purple sunbirds.</t>
   </si>
   <si>
-    <t>When seeking nectar, the Purple-rumped sunbirds engage in frequent hovering at flowers, distinguishing them from purple sunbirds, which generally prefer perching beside flowers. Similar to other sunbirds, they also include small insects and spiders in their diet. Additionally, these sunbirds readily drink from various garden plants as well as wild shrubs.</t>
-  </si>
-  <si>
     <t>INDIAN GOLDEN ORIOLE</t>
   </si>
   <si>
@@ -1006,9 +1003,6 @@
     <t>Distinctive features of these birds include a yellow patch on the wings, yellow outer tail feathers, a black stripe across the eye that creates a masked appearance, and a fleshy pink bill. In contrast, females exhibit a dull greenish-yellow overall coloration with wings in dirty brown/green hues and a completely yellowish tail. Both males and females share a red iris.</t>
   </si>
   <si>
-    <t>Loten's sunbirds have a varied diet, consisting of fruits, nectar, and insects. Their feeding habits make them effective seed dispersers for numerous berry-bearing plants.</t>
-  </si>
-  <si>
     <t>BLACK HEADED ORIOLE</t>
   </si>
   <si>
@@ -1027,9 +1021,6 @@
     <t>The male Black-Hooded Oriole stands out with its striking black and yellow coloration, predominantly yellow plumage, a solid black hood, and black wings and tail center. In contrast, the female is less vibrant, featuring greenish underparts with the distinctive black hood. Young birds resemble females but exhibit dark streaking on the underparts, and their hoods are not entirely black, especially on the throat. The black head of the Black-Hooded Oriole serves as a clear distinction from the Indian golden oriole.. These birds, while potentially shy, may be challenging to spot amid the dappled yellow and green leaves of the canopy. In flight, the black-hooded oriole's movement resembles that of a thrush, characterized by a strong and direct flight with some shallow dips over longer distances. When foraging, the species employs various methods, including foliage-gleaning, wood-gleaning, or sallying.</t>
   </si>
   <si>
-    <t>The Black-Hooded Oriole's adaptable diet, ranging from insects like caterpillars and beetles to fruits and nectar, positions them as important contributors to their ecosystem. Their diverse foraging habits support their roles as predators, pollinators, and seed dispersers, contributing to the overall health and balance of their habitats.</t>
-  </si>
-  <si>
     <t>SPOT BILLED PELICAN</t>
   </si>
   <si>
@@ -1328,6 +1319,18 @@
   </si>
   <si>
     <t>The common kingfisher's primary diet consists mainly of small fish, although it also includes insect larvae and, occasionally, frogs. When perched on a branch or reed above the water, the small bird patiently awaits the sight of a potential prey - a small fish in the water. Upon spotting its target, the kingfisher executes a swift, vertical plunge into the water with its wings retracted. In an attempt to catch the fish, the bird uses its beak before swiftly taking off again. To subdue and prepare its catch, the kingfisher often strikes the fish several times against a branch.</t>
+  </si>
+  <si>
+    <t>During their quest for nectar, they frequently hover around flowers. Similar to other sunbirds, they also consume small insects and spiders. Their drinking habits encompass both garden plants and more untamed shrubs with equal enthusiasm.</t>
+  </si>
+  <si>
+    <t>The Black-Headed Oriole's adaptable diet, ranging from insects like caterpillars and beetles to fruits and nectar, positions them as important contributors to their ecosystem. Their diverse foraging habits support their roles as predators, pollinators, and seed dispersers, contributing to the overall health and balance of their habitats.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The diet of these golden oriole species consists mainly of wild fruits. </t>
+  </si>
+  <si>
+    <t>Little cormorant birds primarily consume fish, occasionally incorporating crustaceans and amphibians into their diet. They engage in diving to capture their prey and resurface to swallow it.</t>
   </si>
 </sst>
 </file>
@@ -1701,8 +1704,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2104,7 +2107,7 @@
         <v>60</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -3852,7 +3855,7 @@
         <v>320</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>321</v>
+        <v>433</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -3874,29 +3877,29 @@
     </row>
     <row r="49" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>323</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>324</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="H49" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="H49" s="4" t="s">
-        <v>327</v>
-      </c>
       <c r="I49" s="4" t="s">
-        <v>328</v>
+        <v>435</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -3918,31 +3921,31 @@
     </row>
     <row r="50" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E50" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="G50" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="H50" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>334</v>
-      </c>
       <c r="I50" s="4" t="s">
-        <v>335</v>
+        <v>434</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -3964,13 +3967,13 @@
     </row>
     <row r="51" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>71</v>
@@ -3980,13 +3983,13 @@
         <v>41</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4008,31 +4011,31 @@
     </row>
     <row r="52" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -4054,13 +4057,13 @@
     </row>
     <row r="53" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>12</v>
@@ -4070,13 +4073,13 @@
         <v>41</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4098,13 +4101,13 @@
     </row>
     <row r="54" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>12</v>
@@ -4114,12 +4117,14 @@
         <v>41</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="I54" s="4"/>
+        <v>354</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>436</v>
+      </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -4140,31 +4145,31 @@
     </row>
     <row r="55" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E55" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="H55" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="I55" s="17" t="s">
         <v>362</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="H55" s="17" t="s">
-        <v>364</v>
-      </c>
-      <c r="I55" s="17" t="s">
-        <v>365</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4186,29 +4191,29 @@
     </row>
     <row r="56" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="H56" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="I56" s="17" t="s">
         <v>369</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>372</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -4230,31 +4235,31 @@
     </row>
     <row r="57" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="I57" s="4" t="s">
         <v>376</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>379</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4276,29 +4281,29 @@
     </row>
     <row r="58" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="I58" s="4" t="s">
         <v>383</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>386</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4320,29 +4325,29 @@
     </row>
     <row r="59" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>389</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>392</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -4364,29 +4369,29 @@
     </row>
     <row r="60" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="I60" s="4" t="s">
         <v>396</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>399</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -4408,29 +4413,29 @@
     </row>
     <row r="61" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -4452,31 +4457,31 @@
     </row>
     <row r="62" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E62" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="H62" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="F62" s="6" t="s">
+      <c r="I62" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>412</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -4498,31 +4503,31 @@
     </row>
     <row r="63" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E63" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="H63" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="I63" s="10" t="s">
         <v>416</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="I63" s="10" t="s">
-        <v>419</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -4544,31 +4549,31 @@
     </row>
     <row r="64" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E64" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="H64" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="I64" s="4" t="s">
         <v>424</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="H64" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>427</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -4590,31 +4595,31 @@
     </row>
     <row r="65" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>

</xml_diff>

<commit_message>
Data corrected according to the national red list. Conservation statuses added to the doc, some images of the site were added and also another minor changes
</commit_message>
<xml_diff>
--- a/uomBirds.xlsx
+++ b/uomBirds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA10236-1603-4D64-8571-A02998526BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D67414-6960-4A45-B0EE-99ABBA9B19D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="441">
   <si>
     <t>Common Name</t>
   </si>
@@ -58,9 +58,6 @@
     <t xml:space="preserve"> Accipitridae</t>
   </si>
   <si>
-    <t>Least Concern</t>
-  </si>
-  <si>
     <t>red backed sea eagle</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>Anhingidae</t>
   </si>
   <si>
-    <t>Near Threatened</t>
-  </si>
-  <si>
     <t>Uncommon breeeding resident in dry lowlands. Very rarely observed in wet lowlands and high hills. Tanks, lakes, larger rivers and lagoons are the preffered habitat.</t>
   </si>
   <si>
@@ -502,9 +496,6 @@
     <t>SPOTTED DOVE</t>
   </si>
   <si>
-    <t>Spilopelia chinensis</t>
-  </si>
-  <si>
     <t>Eastern spotted dove</t>
   </si>
   <si>
@@ -751,9 +742,6 @@
     <t>YELLOW BILLED BABLER</t>
   </si>
   <si>
-    <t>Turdoides affinis</t>
-  </si>
-  <si>
     <t>Leiothrichidae</t>
   </si>
   <si>
@@ -772,9 +760,6 @@
     <t>BROWN HEADED BARBET</t>
   </si>
   <si>
-    <t>Megalaima zeylanica</t>
-  </si>
-  <si>
     <t>Megalaimidae</t>
   </si>
   <si>
@@ -793,9 +778,6 @@
     <t>CEYLON SMALL BARBET</t>
   </si>
   <si>
-    <t>Megalaima rubricapillus</t>
-  </si>
-  <si>
     <t>Crimson fronted barbet, Sri lanka barbet</t>
   </si>
   <si>
@@ -856,9 +838,6 @@
     <t>EASTERN/WESTERN YELLOW WAGTAIL</t>
   </si>
   <si>
-    <t>Motacilla tschutschensis</t>
-  </si>
-  <si>
     <t>Motacillidae</t>
   </si>
   <si>
@@ -931,12 +910,6 @@
     <t>Being insectivorous, brown-breasted flycatchers primarily feed on insects. Their common food items include beetles, caterpillars, flies, and spiders.</t>
   </si>
   <si>
-    <t>INDIAN BLACK ROBIN</t>
-  </si>
-  <si>
-    <t>Copsychus fulicatus</t>
-  </si>
-  <si>
     <t>Observed only once in the courtyard of the chemical engineering department.</t>
   </si>
   <si>
@@ -1117,9 +1090,6 @@
     <t>Loriculus beryllinus</t>
   </si>
   <si>
-    <t>Psittaculidae</t>
-  </si>
-  <si>
     <t>Surrounding areas of university ground and Ceremonial courtyard.</t>
   </si>
   <si>
@@ -1216,9 +1186,6 @@
     <t>PURPLE SWAMPHEN</t>
   </si>
   <si>
-    <t>Porphyrio porphyrio</t>
-  </si>
-  <si>
     <t>Locally common breeding resident in the lowlands. Reedbeds, marshes, paddyfields and weedy tanks are the habitat types which can be easily spotted.</t>
   </si>
   <si>
@@ -1331,13 +1298,58 @@
   </si>
   <si>
     <t>Little cormorant birds primarily consume fish, occasionally incorporating crustaceans and amphibians into their diet. They engage in diving to capture their prey and resurface to swallow it.</t>
+  </si>
+  <si>
+    <t>VU</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>Spilopelia suratensis</t>
+  </si>
+  <si>
+    <t>Western Koel</t>
+  </si>
+  <si>
+    <t>Argya affinis</t>
+  </si>
+  <si>
+    <t>Psilopogon zeylanicus</t>
+  </si>
+  <si>
+    <t>Psilopogon rubricapillus</t>
+  </si>
+  <si>
+    <t>Motacilla tschutschensis/Motacilla tschutschensis</t>
+  </si>
+  <si>
+    <t>INDIAN ROBIN</t>
+  </si>
+  <si>
+    <t>Saxicoloides fulicatus</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>Psittacidae</t>
+  </si>
+  <si>
+    <t>Porphyrio poliocephalus</t>
+  </si>
+  <si>
+    <t>LC*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1367,8 +1379,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1397,6 +1422,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1442,7 +1479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1475,20 +1512,24 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <i/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1704,14 +1745,13 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="1" max="2" width="26.44140625" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="47.77734375" customWidth="1"/>
@@ -1724,7 +1764,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1770,29 +1810,29 @@
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1814,31 +1854,31 @@
     </row>
     <row r="3" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
+      <c r="D3" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1860,29 +1900,29 @@
     </row>
     <row r="4" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
+      <c r="D4" s="26" t="s">
+        <v>426</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1904,31 +1944,31 @@
     </row>
     <row r="5" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
+      <c r="D5" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1950,29 +1990,29 @@
     </row>
     <row r="6" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>12</v>
+      <c r="D6" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1994,31 +2034,31 @@
     </row>
     <row r="7" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="F7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2040,28 +2080,28 @@
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2083,31 +2123,31 @@
     </row>
     <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2129,31 +2169,31 @@
     </row>
     <row r="10" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2175,29 +2215,29 @@
     </row>
     <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>71</v>
+      <c r="D11" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -2219,29 +2259,29 @@
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>12</v>
+      <c r="D12" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="I12" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2263,31 +2303,31 @@
     </row>
     <row r="13" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="F13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2309,31 +2349,31 @@
     </row>
     <row r="14" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="F14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2355,29 +2395,29 @@
     </row>
     <row r="15" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>12</v>
+        <v>88</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -2399,31 +2439,31 @@
     </row>
     <row r="16" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="F16" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="H16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -2445,31 +2485,31 @@
     </row>
     <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="H17" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2491,29 +2531,29 @@
     </row>
     <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>12</v>
+        <v>88</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2535,29 +2575,29 @@
     </row>
     <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>12</v>
+      <c r="D19" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2579,31 +2619,31 @@
     </row>
     <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="D20" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="F20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2625,29 +2665,29 @@
     </row>
     <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>132</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>12</v>
+        <v>126</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2669,29 +2709,29 @@
     </row>
     <row r="22" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>12</v>
+      <c r="D22" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2713,31 +2753,31 @@
     </row>
     <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="D23" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="F23" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="H23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -2759,29 +2799,29 @@
     </row>
     <row r="24" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>152</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>12</v>
+        <v>145</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -2803,31 +2843,31 @@
     </row>
     <row r="25" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="I25" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -2849,31 +2889,31 @@
     </row>
     <row r="26" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="F26" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="I26" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>173</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -2895,31 +2935,31 @@
     </row>
     <row r="27" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -2941,29 +2981,31 @@
     </row>
     <row r="28" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>430</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="6" t="s">
+      <c r="I28" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2985,31 +3027,31 @@
     </row>
     <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="I29" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -3031,31 +3073,31 @@
     </row>
     <row r="30" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="F30" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="I30" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -3077,29 +3119,29 @@
     </row>
     <row r="31" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>200</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>12</v>
+        <v>201</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3121,31 +3163,31 @@
     </row>
     <row r="32" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="F32" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="I32" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3167,29 +3209,29 @@
     </row>
     <row r="33" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>215</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>12</v>
+        <v>216</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>440</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3211,29 +3253,29 @@
     </row>
     <row r="34" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>225</v>
+        <v>221</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>222</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>12</v>
+        <v>216</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="I34" s="17" t="s">
         <v>226</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>229</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3255,29 +3297,29 @@
     </row>
     <row r="35" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>228</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>12</v>
+        <v>229</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3299,29 +3341,29 @@
     </row>
     <row r="36" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>234</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>12</v>
+        <v>235</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>440</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -3343,29 +3385,29 @@
     </row>
     <row r="37" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>12</v>
+        <v>239</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3387,29 +3429,29 @@
     </row>
     <row r="38" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>250</v>
+        <v>245</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>432</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>12</v>
+        <v>246</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -3431,31 +3473,31 @@
     </row>
     <row r="39" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>433</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="I39" s="17" t="s">
         <v>256</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>262</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3477,29 +3519,29 @@
     </row>
     <row r="40" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>264</v>
+        <v>257</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>258</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>12</v>
+        <v>259</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>428</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -3521,29 +3563,29 @@
     </row>
     <row r="41" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>265</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>12</v>
+        <v>266</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3565,29 +3607,29 @@
     </row>
     <row r="42" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>278</v>
+        <v>271</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>434</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>12</v>
+        <v>272</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>440</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3609,29 +3651,29 @@
     </row>
     <row r="43" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>285</v>
+        <v>277</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>278</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>12</v>
+        <v>272</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="6" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3653,29 +3695,29 @@
     </row>
     <row r="44" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>291</v>
+        <v>283</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>284</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>12</v>
+        <v>285</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="19" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -3697,31 +3739,31 @@
     </row>
     <row r="45" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>297</v>
+        <v>289</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>290</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>299</v>
-      </c>
       <c r="G45" s="4" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -3743,29 +3785,29 @@
     </row>
     <row r="46" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>304</v>
+        <v>435</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>436</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>12</v>
+        <v>285</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -3787,29 +3829,29 @@
     </row>
     <row r="47" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>309</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>310</v>
+        <v>300</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>301</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>12</v>
+        <v>302</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>427</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -3831,31 +3873,31 @@
     </row>
     <row r="48" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>317</v>
+        <v>307</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>308</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>320</v>
-      </c>
       <c r="I48" s="4" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -3877,29 +3919,29 @@
     </row>
     <row r="49" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>322</v>
+        <v>312</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>313</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>12</v>
+        <v>314</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>440</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -3921,31 +3963,31 @@
     </row>
     <row r="50" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>328</v>
+        <v>318</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>319</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="H50" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>332</v>
-      </c>
       <c r="I50" s="4" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -3967,29 +4009,29 @@
     </row>
     <row r="51" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>334</v>
+        <v>324</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>325</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>71</v>
+        <v>326</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4011,31 +4053,31 @@
     </row>
     <row r="52" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>340</v>
+        <v>330</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>331</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>12</v>
+        <v>332</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -4057,29 +4099,29 @@
     </row>
     <row r="53" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>347</v>
+        <v>337</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>338</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>12</v>
+        <v>332</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>437</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4101,29 +4143,29 @@
     </row>
     <row r="54" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>352</v>
+        <v>342</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>343</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>12</v>
+        <v>332</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -4145,31 +4187,31 @@
     </row>
     <row r="55" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>356</v>
+        <v>346</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>347</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>12</v>
+        <v>348</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4191,29 +4233,29 @@
     </row>
     <row r="56" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>364</v>
+        <v>354</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>355</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>365</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>12</v>
+        <v>438</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="6" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -4235,31 +4277,31 @@
     </row>
     <row r="57" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>371</v>
+        <v>360</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>361</v>
       </c>
       <c r="C57" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>375</v>
-      </c>
       <c r="I57" s="4" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4281,29 +4323,29 @@
     </row>
     <row r="58" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>378</v>
+        <v>367</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>368</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>12</v>
+        <v>369</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="6" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4325,29 +4367,29 @@
     </row>
     <row r="59" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>385</v>
+        <v>374</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>375</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>12</v>
+        <v>369</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -4369,29 +4411,29 @@
     </row>
     <row r="60" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>391</v>
+        <v>380</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>381</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>12</v>
+        <v>382</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="6" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -4413,29 +4455,29 @@
     </row>
     <row r="61" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>398</v>
+        <v>387</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>439</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>12</v>
+        <v>382</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="6" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -4457,31 +4499,31 @@
     </row>
     <row r="62" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>403</v>
+        <v>391</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>392</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>12</v>
+        <v>393</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>437</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -4503,31 +4545,31 @@
     </row>
     <row r="63" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>411</v>
+        <v>399</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>400</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="H63" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="H63" s="4" t="s">
-        <v>415</v>
-      </c>
       <c r="I63" s="10" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -4549,31 +4591,31 @@
     </row>
     <row r="64" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>418</v>
+        <v>406</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>407</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>12</v>
+        <v>408</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>427</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -4595,31 +4637,31 @@
     </row>
     <row r="65" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>426</v>
+        <v>414</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>415</v>
       </c>
       <c r="C65" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="D65" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="D65" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="E65" s="4" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -30816,11 +30858,7 @@
       <c r="Z1000" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B3:B1000">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Magpie robin and Ind.g.oriole locations updated./ Added '-' to the bird names and some other minor changes
</commit_message>
<xml_diff>
--- a/uomBirds.xlsx
+++ b/uomBirds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D67414-6960-4A45-B0EE-99ABBA9B19D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBEA2BD-E4D0-4739-B47E-BAF81D273834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="440">
   <si>
     <t>Common Name</t>
   </si>
@@ -58,9 +58,6 @@
     <t xml:space="preserve"> Accipitridae</t>
   </si>
   <si>
-    <t>red backed sea eagle</t>
-  </si>
-  <si>
     <t>Most commonly can  be observed during flight in anywhere in the university sky. Perched specimen can be spotted near the university ground premises and the bolgoda lakeside trees.</t>
   </si>
   <si>
@@ -112,15 +109,9 @@
     <t>Primarily larvae, pupae, and honeycombs of social wasps and bees, occasionally supplemented with cicadas, small birds, reptiles, and frogs. They dig up wasp nests with their strong talons and long beak, adapted for extracting prey from combs.</t>
   </si>
   <si>
-    <t>WHITE BELLIED SEA EAGLE</t>
-  </si>
-  <si>
     <t>Haliaeetus leucogaster</t>
   </si>
   <si>
-    <t>white breasted sea eagle</t>
-  </si>
-  <si>
     <t>Around the university ground and the boart yard area</t>
   </si>
   <si>
@@ -133,9 +124,6 @@
     <t>Primarily fish, scavenged carrion, and occasionally reptiles and crustaceans. They hunt by soaring and diving, snatching prey from the water's surface.</t>
   </si>
   <si>
-    <t>STORK BILLED KINGFISHER</t>
-  </si>
-  <si>
     <t>Pelargopsis capensis</t>
   </si>
   <si>
@@ -154,15 +142,9 @@
     <t>Mainly consists of fresh water fish speices, crustatians, frogs and sometimes small rodents.</t>
   </si>
   <si>
-    <t>WHITE BRESTED KINGFISHER</t>
-  </si>
-  <si>
     <t>Halcyon smyrnensis</t>
   </si>
   <si>
-    <t>white throated kingfisher</t>
-  </si>
-  <si>
     <t>Common breeding resident that is found throughout the Island. Can be observed in open areas,cultivation,gardens and wetlands. Argubly the most common kingfisher species in Sri Lanka.</t>
   </si>
   <si>
@@ -172,9 +154,6 @@
     <t>This predator primarily targets a diverse range of prey, including large crustaceans, insects, earthworms, rodents, lizards, snakes, fish, and frogs. There have been reported instances of predation on small birds, such as the Indian white-eye, chicks of red-wattled lapwings, sparrows, and munias. Notably, the young of this species are predominantly fed on invertebrates.</t>
   </si>
   <si>
-    <t>LESSER PIED KINGFISHER</t>
-  </si>
-  <si>
     <t>Ceryle rudis</t>
   </si>
   <si>
@@ -337,15 +316,9 @@
     <t>Mainly consists of crustaceans, aquatic insects, fishes, tadpoles and sometimes leeches. Outside wetlands, these herons regularly feed on insects (including crickets, dragonflies and bees)</t>
   </si>
   <si>
-    <t>BLACK CROWNED NIGHT HERON</t>
-  </si>
-  <si>
     <t>Nycticorax nycticorax</t>
   </si>
   <si>
-    <t>Black capped night heron</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boart yard and the surrounding marshy areas of the Bolgoda lake. </t>
   </si>
   <si>
@@ -373,9 +346,6 @@
     <t>Grey herons are carnivores, primarily piscivores, and their main diet consists of fish. However, their feeding habits can vary with the season and availability of prey. They may also consume amphibians, crustaceans, aquatic invertebrates, mollusks, snakes, small birds, rodents, and occasionally, certain plants.</t>
   </si>
   <si>
-    <t>RED WATTLED LAPWING</t>
-  </si>
-  <si>
     <t>Vanellus indicus</t>
   </si>
   <si>
@@ -403,9 +373,6 @@
     <t>Ciconiidae</t>
   </si>
   <si>
-    <t>Asian openbill stork</t>
-  </si>
-  <si>
     <t>Fairly common breeding resident in lowlands, can be found in small numbers along rivers in interior wet zone and on lakes and rivers up to lower hills. Marshes, tanks,lakes,rivers and lagoons are the preffered habitats.</t>
   </si>
   <si>
@@ -520,9 +487,6 @@
     <t>Corvidae</t>
   </si>
   <si>
-    <t>Indian/grey necked/Ceylon/Colombo crow</t>
-  </si>
-  <si>
     <t xml:space="preserve">Throughout the university. </t>
   </si>
   <si>
@@ -595,9 +559,6 @@
     <t>Mainly  insects, caterpillars, snails, and small vertebrates. Also known to eat bird eggs, nestlings, fruits, and seeds.</t>
   </si>
   <si>
-    <t>PALE BILLED FLOWERPECKER</t>
-  </si>
-  <si>
     <t>Dicaeum erythrorhynchos</t>
   </si>
   <si>
@@ -619,9 +580,6 @@
     <t xml:space="preserve"> feeds on nectar and berries</t>
   </si>
   <si>
-    <t>WHITE BELLIED DRONGO</t>
-  </si>
-  <si>
     <t>Dicrurus caerulescens</t>
   </si>
   <si>
@@ -640,18 +598,12 @@
     <t>While primarily insectivorous, these birds display opportunistic behavior and are known to prey on small birds. Similar to other drongos, they utilize their feet when handling prey. Additionally, they have been observed taking advantage of insects attracted to artificial lights during the late dusk period.</t>
   </si>
   <si>
-    <t>SCALY BREASTED MUNIA</t>
-  </si>
-  <si>
     <t>Lonchura punctulata</t>
   </si>
   <si>
     <t>Estrildidae</t>
   </si>
   <si>
-    <t>Spotted munia, Spice finch</t>
-  </si>
-  <si>
     <t>Trees between Sumanadasa building and the University ground. Bushy areas behind the Main building of Department of Civil Engineering, Open areas around around Lagan and Deparment of textile and apparel engineering.</t>
   </si>
   <si>
@@ -703,9 +655,6 @@
     <t>Mostly insectivorous, taking flying insects on the wing.</t>
   </si>
   <si>
-    <t>PHEASANT TAILED JACANA</t>
-  </si>
-  <si>
     <t>Hydrophasianus chirurgus</t>
   </si>
   <si>
@@ -739,9 +688,6 @@
     <t xml:space="preserve"> Small fish, shrimp, and other marine invertebrates. They hunt by dipping their bills into the water while hovering or flying low over the surface.</t>
   </si>
   <si>
-    <t>YELLOW BILLED BABLER</t>
-  </si>
-  <si>
     <t>Leiothrichidae</t>
   </si>
   <si>
@@ -757,9 +703,6 @@
     <t>As an omnivore, this species has a varied diet that includes insects, spiders, small fruits, grains, nectar, and occasionally, lizards or scavenged scraps of food from human habitations.</t>
   </si>
   <si>
-    <t>BROWN HEADED BARBET</t>
-  </si>
-  <si>
     <t>Megalaimidae</t>
   </si>
   <si>
@@ -778,9 +721,6 @@
     <t>CEYLON SMALL BARBET</t>
   </si>
   <si>
-    <t>Crimson fronted barbet, Sri lanka barbet</t>
-  </si>
-  <si>
     <t>Ceremonial Courtyard area</t>
   </si>
   <si>
@@ -793,9 +733,6 @@
     <t>Mainly consists of fruits and insects.</t>
   </si>
   <si>
-    <t>BLUE TAILED BEE EATER</t>
-  </si>
-  <si>
     <t>Merops philippinus</t>
   </si>
   <si>
@@ -889,9 +826,6 @@
     <t>As carnivores, specifically insectivores, their primary diet comprises insects and other invertebrates. On occasion, they may also consume flower nectar, geckos, leeches, centipedes, and even fish.</t>
   </si>
   <si>
-    <t>BROWN BREASTED FLYCATCHER</t>
-  </si>
-  <si>
     <t>Muscicapa muttui</t>
   </si>
   <si>
@@ -922,9 +856,6 @@
     <t>Their primary diet consists mainly of insects, although they are also known to consume frogs and lizards, particularly when feeding their young at the nest. These birds may engage in late evening foraging, targeting insects drawn to lights during this time.</t>
   </si>
   <si>
-    <t>PURPLE RUMPED SUNBIRD</t>
-  </si>
-  <si>
     <t>Leptocoma zeylonica</t>
   </si>
   <si>
@@ -967,24 +898,15 @@
     <t>Oriolidae</t>
   </si>
   <si>
-    <t>Oserved only once and it was in the greenery behind the Library</t>
-  </si>
-  <si>
     <t>Rare winter migrant to lowlands and lower hills. Solitary and can be seen in wooded areas.</t>
   </si>
   <si>
     <t>Distinctive features of these birds include a yellow patch on the wings, yellow outer tail feathers, a black stripe across the eye that creates a masked appearance, and a fleshy pink bill. In contrast, females exhibit a dull greenish-yellow overall coloration with wings in dirty brown/green hues and a completely yellowish tail. Both males and females share a red iris.</t>
   </si>
   <si>
-    <t>BLACK HEADED ORIOLE</t>
-  </si>
-  <si>
     <t>Oriolus xanthornus</t>
   </si>
   <si>
-    <t>Black hooded oriole</t>
-  </si>
-  <si>
     <t>Trees around the Library, Kaju kele and around the trees of Building of Faculty of Architecture.</t>
   </si>
   <si>
@@ -994,9 +916,6 @@
     <t>The male Black-Hooded Oriole stands out with its striking black and yellow coloration, predominantly yellow plumage, a solid black hood, and black wings and tail center. In contrast, the female is less vibrant, featuring greenish underparts with the distinctive black hood. Young birds resemble females but exhibit dark streaking on the underparts, and their hoods are not entirely black, especially on the throat. The black head of the Black-Hooded Oriole serves as a clear distinction from the Indian golden oriole.. These birds, while potentially shy, may be challenging to spot amid the dappled yellow and green leaves of the canopy. In flight, the black-hooded oriole's movement resembles that of a thrush, characterized by a strong and direct flight with some shallow dips over longer distances. When foraging, the species employs various methods, including foliage-gleaning, wood-gleaning, or sallying.</t>
   </si>
   <si>
-    <t>SPOT BILLED PELICAN</t>
-  </si>
-  <si>
     <t>Pelecanus philippensis</t>
   </si>
   <si>
@@ -1102,9 +1021,6 @@
     <t>Their natural diet consists mainly of fruits; particularly wild figs, guava and berries, as well as flower buds and blossoms. Also feeds onnectar and seeds.</t>
   </si>
   <si>
-    <t>ROSE RINGED PARAKEET</t>
-  </si>
-  <si>
     <t>Psittacula krameri</t>
   </si>
   <si>
@@ -1123,9 +1039,6 @@
     <t>usually feed on buds, fruits, vegetables, nuts, berries, and seeds.</t>
   </si>
   <si>
-    <t>RED VENTED BULBUL</t>
-  </si>
-  <si>
     <t>Pycnonotus cafer</t>
   </si>
   <si>
@@ -1144,9 +1057,6 @@
     <t>Their diet encompasses a variety of food sources, including fruits, flower petals, nectar, and insects. Additionally, they occasionally consume house geckos.</t>
   </si>
   <si>
-    <t>WHITE BROWED BULBUL</t>
-  </si>
-  <si>
     <t>Pycnonotus luteolus</t>
   </si>
   <si>
@@ -1162,9 +1072,6 @@
     <t>They search for food within bushes, where they primarily feed on a diet consisting of fruit, nectar, and insects.</t>
   </si>
   <si>
-    <t>WHITE BREASTED WATERHEN</t>
-  </si>
-  <si>
     <t>Amaurornis phoenicurus</t>
   </si>
   <si>
@@ -1225,9 +1132,6 @@
     <t>Otus bakkamoena</t>
   </si>
   <si>
-    <t>Collared scops owl</t>
-  </si>
-  <si>
     <t>Can be observed in seetha gangula area at night</t>
   </si>
   <si>
@@ -1264,9 +1168,6 @@
     <t>Being omnivorous, this species has a diverse diet that includes insects, arachnids, crustaceans, reptiles, small mammals, seeds, grains, fruits, and discarded waste from human habitation.</t>
   </si>
   <si>
-    <t>BLACK HEADED IBIS</t>
-  </si>
-  <si>
     <t>Threskiornis melanocephalus</t>
   </si>
   <si>
@@ -1343,6 +1244,102 @@
   </si>
   <si>
     <t>LC*</t>
+  </si>
+  <si>
+    <t>Oserved only once and it was in the area behind the main building of the Department of Civil Engineering.</t>
+  </si>
+  <si>
+    <t>Observed around the TMLE building and the building of Faculty of IT.</t>
+  </si>
+  <si>
+    <t>WHITE-BELLIED SEA EAGLE</t>
+  </si>
+  <si>
+    <t>STORK-BILLED KINGFISHER</t>
+  </si>
+  <si>
+    <t>WHITE-BRESTED KINGFISHER</t>
+  </si>
+  <si>
+    <t>LESSER-PIED KINGFISHER</t>
+  </si>
+  <si>
+    <t>BLACK-CROWNED NIGHT HERON</t>
+  </si>
+  <si>
+    <t>RED-WATTLED LAPWING</t>
+  </si>
+  <si>
+    <t>PALE-BILLED FLOWERPECKER</t>
+  </si>
+  <si>
+    <t>WHITE-BELLIED DRONGO</t>
+  </si>
+  <si>
+    <t>SCALY-BREASTED MUNIA</t>
+  </si>
+  <si>
+    <t>PHEASANT-TAILED JACANA</t>
+  </si>
+  <si>
+    <t>YELLOW-BILLED BABLER</t>
+  </si>
+  <si>
+    <t>BROWN-HEADED BARBET</t>
+  </si>
+  <si>
+    <t>BLUE-TAILED BEE EATER</t>
+  </si>
+  <si>
+    <t>BROWN-BREASTED FLYCATCHER</t>
+  </si>
+  <si>
+    <t>PURPLE-RUMPED SUNBIRD</t>
+  </si>
+  <si>
+    <t>BLACK-HEADED ORIOLE</t>
+  </si>
+  <si>
+    <t>SPOT-BILLED PELICAN</t>
+  </si>
+  <si>
+    <t>ROSE-RINGED PARAKEET</t>
+  </si>
+  <si>
+    <t>RED-VENTED BULBUL</t>
+  </si>
+  <si>
+    <t>WHITE-BROWED BULBUL</t>
+  </si>
+  <si>
+    <t>WHITE-BREASTED WATERHEN</t>
+  </si>
+  <si>
+    <t>BLACK-HEADED IBIS</t>
+  </si>
+  <si>
+    <t>Collared-scops owl</t>
+  </si>
+  <si>
+    <t>Crimson-fronted barbet, Sri lanka barbet</t>
+  </si>
+  <si>
+    <t>Spotted-munia, Spice finch</t>
+  </si>
+  <si>
+    <t>grey-necked crow</t>
+  </si>
+  <si>
+    <t>Black-capped night heron</t>
+  </si>
+  <si>
+    <t>white-throated kingfisher</t>
+  </si>
+  <si>
+    <t>white-breasted sea eagle</t>
+  </si>
+  <si>
+    <t>red-backed sea eagle</t>
   </si>
 </sst>
 </file>
@@ -1514,17 +1511,17 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1746,7 +1743,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1817,22 +1814,22 @@
         <v>11</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -1854,31 +1851,31 @@
     </row>
     <row r="3" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1900,29 +1897,29 @@
     </row>
     <row r="4" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>426</v>
+        <v>393</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1944,31 +1941,31 @@
     </row>
     <row r="5" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>410</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1990,29 +1987,29 @@
     </row>
     <row r="6" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>37</v>
+        <v>411</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -2034,31 +2031,31 @@
     </row>
     <row r="7" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>44</v>
+        <v>412</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>437</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2080,28 +2077,28 @@
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>50</v>
+        <v>413</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2123,31 +2120,31 @@
     </row>
     <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>421</v>
+        <v>388</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2169,31 +2166,31 @@
     </row>
     <row r="10" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2215,29 +2212,29 @@
     </row>
     <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -2259,29 +2256,29 @@
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2303,31 +2300,31 @@
     </row>
     <row r="13" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="F13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="H13" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2349,31 +2346,31 @@
     </row>
     <row r="14" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2395,29 +2392,29 @@
     </row>
     <row r="15" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -2439,31 +2436,31 @@
     </row>
     <row r="16" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -2485,31 +2482,31 @@
     </row>
     <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>105</v>
+        <v>414</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>107</v>
+        <v>436</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2531,29 +2528,29 @@
     </row>
     <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2575,29 +2572,29 @@
     </row>
     <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>117</v>
+        <v>415</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2619,31 +2616,29 @@
     </row>
     <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>427</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>127</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2665,29 +2660,29 @@
     </row>
     <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2709,29 +2704,29 @@
     </row>
     <row r="22" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2753,31 +2748,31 @@
     </row>
     <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>428</v>
+        <v>395</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -2799,29 +2794,29 @@
     </row>
     <row r="24" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="6" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -2843,31 +2838,31 @@
     </row>
     <row r="25" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>429</v>
+        <v>396</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -2889,31 +2884,31 @@
     </row>
     <row r="26" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>166</v>
+        <v>435</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -2935,31 +2930,31 @@
     </row>
     <row r="27" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -2981,31 +2976,31 @@
     </row>
     <row r="28" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>430</v>
+        <v>397</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -3027,31 +3022,31 @@
     </row>
     <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -3073,31 +3068,31 @@
     </row>
     <row r="30" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>191</v>
+        <v>416</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -3119,29 +3114,29 @@
     </row>
     <row r="31" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>199</v>
+        <v>417</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="16" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3163,31 +3158,31 @@
     </row>
     <row r="32" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>206</v>
+        <v>418</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>209</v>
+        <v>434</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3209,29 +3204,29 @@
     </row>
     <row r="33" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="16" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3253,29 +3248,29 @@
     </row>
     <row r="34" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="6" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3297,29 +3292,29 @@
     </row>
     <row r="35" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>227</v>
+        <v>419</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3341,29 +3336,29 @@
     </row>
     <row r="36" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -3385,29 +3380,29 @@
     </row>
     <row r="37" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>239</v>
+        <v>420</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>431</v>
+        <v>398</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="6" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3429,29 +3424,29 @@
     </row>
     <row r="38" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>245</v>
+        <v>421</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>432</v>
+        <v>399</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="6" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -3473,31 +3468,31 @@
     </row>
     <row r="39" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="B39" s="27" t="s">
+        <v>400</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>427</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>252</v>
-      </c>
       <c r="F39" s="6" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3519,29 +3514,29 @@
     </row>
     <row r="40" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>257</v>
+        <v>422</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>428</v>
+        <v>395</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -3563,29 +3558,29 @@
     </row>
     <row r="41" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3607,29 +3602,29 @@
     </row>
     <row r="42" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>434</v>
+        <v>401</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3651,29 +3646,29 @@
     </row>
     <row r="43" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="6" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3695,29 +3690,29 @@
     </row>
     <row r="44" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="19" t="s">
-        <v>273</v>
+        <v>409</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -3739,31 +3734,31 @@
     </row>
     <row r="45" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>289</v>
+        <v>423</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -3785,29 +3780,29 @@
     </row>
     <row r="46" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>435</v>
+        <v>402</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>436</v>
+        <v>403</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4" t="s">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>299</v>
+        <v>277</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -3829,29 +3824,29 @@
     </row>
     <row r="47" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>300</v>
+        <v>424</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -3873,31 +3868,31 @@
     </row>
     <row r="48" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>422</v>
+        <v>389</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -3919,29 +3914,29 @@
     </row>
     <row r="49" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>440</v>
+        <v>407</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6" t="s">
-        <v>315</v>
+        <v>408</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>424</v>
+        <v>391</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -3963,31 +3958,29 @@
     </row>
     <row r="50" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>318</v>
+        <v>425</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>427</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>320</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="E50" s="4"/>
       <c r="F50" s="6" t="s">
-        <v>321</v>
+        <v>295</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>322</v>
+        <v>296</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>423</v>
+        <v>390</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -4009,29 +4002,29 @@
     </row>
     <row r="51" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>324</v>
+        <v>426</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4053,31 +4046,31 @@
     </row>
     <row r="52" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -4099,29 +4092,29 @@
     </row>
     <row r="53" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4143,29 +4136,29 @@
     </row>
     <row r="54" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>425</v>
+        <v>392</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -4187,31 +4180,31 @@
     </row>
     <row r="55" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4233,29 +4226,29 @@
     </row>
     <row r="56" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>355</v>
+        <v>328</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>438</v>
+        <v>405</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="6" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -4277,31 +4270,31 @@
     </row>
     <row r="57" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>360</v>
+        <v>427</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>438</v>
+        <v>405</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>364</v>
+        <v>336</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4323,29 +4316,29 @@
     </row>
     <row r="58" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>367</v>
+        <v>428</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="6" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4367,29 +4360,29 @@
     </row>
     <row r="59" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>374</v>
+        <v>429</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>375</v>
+        <v>345</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>378</v>
+        <v>348</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>379</v>
+        <v>349</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -4411,29 +4404,29 @@
     </row>
     <row r="60" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>381</v>
+        <v>350</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>382</v>
+        <v>351</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="6" t="s">
-        <v>383</v>
+        <v>352</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>384</v>
+        <v>353</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>385</v>
+        <v>354</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>386</v>
+        <v>355</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -4455,29 +4448,29 @@
     </row>
     <row r="61" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>387</v>
+        <v>356</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>439</v>
+        <v>406</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>382</v>
+        <v>351</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="6" t="s">
-        <v>383</v>
+        <v>352</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>388</v>
+        <v>357</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>389</v>
+        <v>358</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>390</v>
+        <v>359</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -4499,31 +4492,31 @@
     </row>
     <row r="62" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>392</v>
+        <v>361</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>397</v>
+        <v>366</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>398</v>
+        <v>367</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -4545,31 +4538,31 @@
     </row>
     <row r="63" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>399</v>
+        <v>368</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>401</v>
+        <v>432</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>402</v>
+        <v>370</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>403</v>
+        <v>371</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>404</v>
+        <v>372</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>405</v>
+        <v>373</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -4591,31 +4584,31 @@
     </row>
     <row r="64" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>406</v>
+        <v>374</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>407</v>
+        <v>375</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>408</v>
+        <v>376</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>409</v>
+        <v>377</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>410</v>
+        <v>378</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>411</v>
+        <v>379</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>412</v>
+        <v>380</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -4637,31 +4630,31 @@
     </row>
     <row r="65" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>415</v>
+        <v>382</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>416</v>
+        <v>383</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>427</v>
+        <v>394</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>417</v>
+        <v>384</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>418</v>
+        <v>385</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>419</v>
+        <v>386</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>420</v>
+        <v>387</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>

</xml_diff>

<commit_message>
Updated the xlsx adding new birds and updating locations according to final data collection sessions. Have to add D/H/R data for new birds
</commit_message>
<xml_diff>
--- a/uomBirds.xlsx
+++ b/uomBirds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBEA2BD-E4D0-4739-B47E-BAF81D273834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB9ED1E-7315-47E9-A7F1-EE080D63A3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="482">
   <si>
     <t>Common Name</t>
   </si>
@@ -79,9 +79,6 @@
     <t>little banded goshawk</t>
   </si>
   <si>
-    <t>Trees around the Sumanadasa building and the Lagan.</t>
-  </si>
-  <si>
     <t>A common breeding resident throughout the entire island. Can be observed in both open country and in dense forest. Specially can be observed in close proximity with residential areas too.</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>Pernis ptilorhynchus</t>
   </si>
   <si>
-    <t>Edges of the university ground</t>
-  </si>
-  <si>
     <t>Fairly rare breeding resident and the population much increased by the winter migrants. Occurs throughout the Island. Mostly observed in well-wooded areas.</t>
   </si>
   <si>
@@ -304,9 +298,6 @@
     <t>Paddybird</t>
   </si>
   <si>
-    <t>Around the edges of the Bolgoda lake and open grassy areas throughout the university.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Can be found around the edges of marshes, coastal lagoons and freshwater wetlands. Common breeding residents that can be found all throughout Sri Lanka and numerous winter migrants appear to arrive all over the country. </t>
   </si>
   <si>
@@ -352,9 +343,6 @@
     <t>Charadriidae</t>
   </si>
   <si>
-    <t>Observed in the university ground premises and in the open area in front of Department of Civil Engineering.</t>
-  </si>
-  <si>
     <t>Common breeding resident throughout the island but somewhat rare in hills. Can be commonly spotted in open flat grounds located in the near viscinity of water.</t>
   </si>
   <si>
@@ -406,9 +394,6 @@
     <t>Cisticolidae</t>
   </si>
   <si>
-    <t>Mostly observed in the bushes and trees near library area in the side of Kaju kele. Also observed in the university ground at the side of lagan.</t>
-  </si>
-  <si>
     <t>Common breeding resident throughout Sri Lanka. Can be seen in forest wooded areas, adn trees in villages and town gardens.</t>
   </si>
   <si>
@@ -466,9 +451,6 @@
     <t>Eastern spotted dove</t>
   </si>
   <si>
-    <t>Almost throughout the university premises.</t>
-  </si>
-  <si>
     <t>Very common breeding resident found throughout the island except the high hills. Cultivation, gardens and the open forests are the preffered habitat and usually avoids interior of dense wet forests.</t>
   </si>
   <si>
@@ -526,9 +508,6 @@
     <t>Cuculidae</t>
   </si>
   <si>
-    <t>Can be seen throughout the university where there are trees.</t>
-  </si>
-  <si>
     <t>Common breeding resident from lowland to midhills. Forests, open woodlands gardens and cultivations are the habitats that mostly preffered.</t>
   </si>
   <si>
@@ -604,9 +583,6 @@
     <t>Estrildidae</t>
   </si>
   <si>
-    <t>Trees between Sumanadasa building and the University ground. Bushy areas behind the Main building of Department of Civil Engineering, Open areas around around Lagan and Deparment of textile and apparel engineering.</t>
-  </si>
-  <si>
     <t>Common breeding resident thoughout the Island. Cultivation and open gardens are the preffered habitat.</t>
   </si>
   <si>
@@ -625,9 +601,6 @@
     <t>Hirundinidae</t>
   </si>
   <si>
-    <t>Can be seen in flight around the university ground in the season.</t>
-  </si>
-  <si>
     <t>Three recognised subspecies. H.r. gutturalis is a very common winter migrant. H.r.rustica is a rare and uncommon migrant. H.r.tyleri is a very rare but very regular migrant. Often can be seen in open country and towns near water.</t>
   </si>
   <si>
@@ -643,9 +616,6 @@
     <t>Cecropis hyperythra</t>
   </si>
   <si>
-    <t>Can be seen in flight around the university ground.</t>
-  </si>
-  <si>
     <t>Uncommon breeding resident throughout Sri Lanka. Open areas at forest fringe, plantations,human habitation, grasslands and paddyfields are the preffered habitat of the ceylon swallow.</t>
   </si>
   <si>
@@ -691,9 +661,6 @@
     <t>Leiothrichidae</t>
   </si>
   <si>
-    <t>Lagan and surroundings and also in the area in front of the Auditorium building of Faculty of Architecture.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Common breeding resident from lowlands up to mid hills. uncommon and local further in higher hills. Mostly being on the ground can be seen in wooded areas and trees in villages and town gardens. Avoids forests in wet zone and adjoining hills. </t>
   </si>
   <si>
@@ -706,9 +673,6 @@
     <t>Megalaimidae</t>
   </si>
   <si>
-    <t xml:space="preserve">Area behind the Steel building and In Kaju kele. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Common breeding resident from lowlands up to mid hills. Uncommon but recoreded in higher hills. Forests,open woods.gardens and trees in cultivation are the habitat which can be observed mostly. </t>
   </si>
   <si>
@@ -721,9 +685,6 @@
     <t>CEYLON SMALL BARBET</t>
   </si>
   <si>
-    <t>Ceremonial Courtyard area</t>
-  </si>
-  <si>
     <t>Endemic, fairly common locally from wet lowlands up to mid hills. Uncommon but recorded in dry zone. Forests and the open wooded country is the preffered habitat.</t>
   </si>
   <si>
@@ -739,9 +700,6 @@
     <t>Meropidae</t>
   </si>
   <si>
-    <t>University ground, On and around Sumanadasa Building, Can be seen in flight around the trees of  ENTC and Department of Architecture.</t>
-  </si>
-  <si>
     <t>Farily common winter migrants throughout the Island.. Small flocks do breed on eastern dry lowlands. Open areas and the forests are the preffered habitat.</t>
   </si>
   <si>
@@ -760,9 +718,6 @@
     <t>Monarchidae</t>
   </si>
   <si>
-    <t>Observed in Kaju kele area and the tree tops near Department of Civil Engineering.</t>
-  </si>
-  <si>
     <t>Two recognised subspecies. One being(T.p.ceylonensis) a farily common breeding resident found in dry lowlands and adjoining dy lower hills. The other(T.p.paradisi) is a farily common winter migrant througout. Open forests,groves and town gardens are the habitat where mostly can be spotted.</t>
   </si>
   <si>
@@ -778,9 +733,6 @@
     <t>Motacillidae</t>
   </si>
   <si>
-    <t>Around the university ground premises.</t>
-  </si>
-  <si>
     <t>Common winter migrant to Sri Lanka. Can be observed in damp grasslands and marshes.</t>
   </si>
   <si>
@@ -796,9 +748,6 @@
     <t>Anthus rufulus</t>
   </si>
   <si>
-    <t>Observed in the ground premises in near viscinity of Lagan.</t>
-  </si>
-  <si>
     <t>Farily common breeding resident throughout the country. Grasslands and low scrub are the preffered habitat.</t>
   </si>
   <si>
@@ -862,9 +811,6 @@
     <t>Nectariniidae</t>
   </si>
   <si>
-    <t>Many areas where there are flowers present including the surrounding area of Department of FD &amp; PD. Also observed in the trees around the Bhavana and Trees of Ceremonial courtyard.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Common breeding resident in lowlands and up to mid hills. Rare in areas above that. Cultivation,gardens and forest are the places for look for. </t>
   </si>
   <si>
@@ -907,9 +853,6 @@
     <t>Oriolus xanthornus</t>
   </si>
   <si>
-    <t>Trees around the Library, Kaju kele and around the trees of Building of Faculty of Architecture.</t>
-  </si>
-  <si>
     <t>fairly common breeding resident found in lowlands up to mid hills. Forests,wooded areas and trees in villages and town gardens are the habitats where can be easily seen.</t>
   </si>
   <si>
@@ -991,9 +934,6 @@
     <t>Red-backed flameback,Sri Lanka red-backed woodpecker, Black-rumped flameback</t>
   </si>
   <si>
-    <t>Woody areas around the department of Architecture and Lagan.</t>
-  </si>
-  <si>
     <t>Fairly common breeding resident. The southern red-backed race (psarodes) is being the recorded subspecies in the university premises. Forests,coconut plantations and trees in open country are the areas where can be easily observed.</t>
   </si>
   <si>
@@ -1027,9 +967,6 @@
     <t>Indian ringneck, Kramer parrot</t>
   </si>
   <si>
-    <t>Can be seen in flight at evenings in the university ground premises.</t>
-  </si>
-  <si>
     <t>Common breeding resident from lowlands to midhills and a small population recorded in higer hills. Forests and wooded areas by villages and towns are the preffered habittat. Can be observed even in densely populated areas aswell.</t>
   </si>
   <si>
@@ -1045,9 +982,6 @@
     <t>Pycnonotidae</t>
   </si>
   <si>
-    <t>Throughout the university where there are greenery.</t>
-  </si>
-  <si>
     <t>Very common breeding resident that can be seen all around the country. Easy to spot in forest fringe, open forest, cultivated lands and trees in habitation.  Avoid interior of thick forests in wet zone.</t>
   </si>
   <si>
@@ -1132,9 +1066,6 @@
     <t>Otus bakkamoena</t>
   </si>
   <si>
-    <t>Can be observed in seetha gangula area at night</t>
-  </si>
-  <si>
     <t>Fairly common breeding resident found throughout the entire Island. uncommon in the higher hills. avoid interior of wet evergreen forests and typically found inside well wooded areas and residantial gardens of villages and towns.</t>
   </si>
   <si>
@@ -1156,9 +1087,6 @@
     <t>Indian myna</t>
   </si>
   <si>
-    <t>Can be seen throughout the university including inside the goda and goda uda canteen buildings.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Common breeding throughout. Forest edges, trees in open areas, village and town gardens are the places to look for. </t>
   </si>
   <si>
@@ -1246,12 +1174,6 @@
     <t>LC*</t>
   </si>
   <si>
-    <t>Oserved only once and it was in the area behind the main building of the Department of Civil Engineering.</t>
-  </si>
-  <si>
-    <t>Observed around the TMLE building and the building of Faculty of IT.</t>
-  </si>
-  <si>
     <t>WHITE-BELLIED SEA EAGLE</t>
   </si>
   <si>
@@ -1340,6 +1262,210 @@
   </si>
   <si>
     <t>red-backed sea eagle</t>
+  </si>
+  <si>
+    <t>Oserved only once and it was in the wooded area behind the main library building.</t>
+  </si>
+  <si>
+    <t>Can be seen; perched on trees around the ground and in Kaju kele and in flight at Boat yard area.</t>
+  </si>
+  <si>
+    <t>Edges of the university ground, Boat Yard and the surrounding trees.</t>
+  </si>
+  <si>
+    <t>Boart yard and the surrounding areas of Bolgoda lake.</t>
+  </si>
+  <si>
+    <t>Can be seen in near the ground, hostels and farily common in boat yard and Kaju Kele.</t>
+  </si>
+  <si>
+    <t>Surrounding woody areas of the university ground and open banks of Bolgoda lake near boat yard.</t>
+  </si>
+  <si>
+    <t>Boat yard and the surrounding areas of Bolgoda lake.</t>
+  </si>
+  <si>
+    <t>Boart yard and the surrounding areas of Bolgoda lake. Mostly observed in flight.</t>
+  </si>
+  <si>
+    <t>Observed very commonly in the university ground premises.</t>
+  </si>
+  <si>
+    <t>Boart yard and the trees of the surrounding areas of Bolgoda lake.</t>
+  </si>
+  <si>
+    <t>Boart yard and the surrounding areas of Bolgoda lake. Documented only once.</t>
+  </si>
+  <si>
+    <t>Mostly observed in the bushes and trees in the side of Kaju kele. Also observed in the university ground at the side of lagan. Faily common throughout the university premises.</t>
+  </si>
+  <si>
+    <t>Almost all throughout the university premises.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throughout the university. Specially in the ground premises. </t>
+  </si>
+  <si>
+    <t>Can be seen throughout the university where there are trees. Common in Kaju Kele and Boat yard area.</t>
+  </si>
+  <si>
+    <t>Trees between Sumanadasa building and the University ground. Bushy areas behind the Main building of Department of Civil Engineering, Open areas around around Lagan and Deparment of textile and apparel engineering and inside Kaju Kele.</t>
+  </si>
+  <si>
+    <t>Can be seen in flight around the university ground and at Bolgoda lake near boat yard in the season.</t>
+  </si>
+  <si>
+    <t>Can be seen in flight around the university ground and near Boat yard.</t>
+  </si>
+  <si>
+    <t>Very common almost all thoughout the university.Lagan,Play ground premises, Open areas in Kaju kele and also in the area in front of the Auditorium building of Faculty of Architecture.</t>
+  </si>
+  <si>
+    <t>Fairly Common to see in Kaju kele. Also can be spotted in the Lagan area and the Play ground premises.</t>
+  </si>
+  <si>
+    <t>Observed in Ceremonial Courtyard, Kaju Kele and "Thummulla" area. Mostly found in Kaju kele.</t>
+  </si>
+  <si>
+    <t>University ground, On and around Sumanadasa Building, Boat yard, Open areas of Kaju kele. Also can be seen around the buildings/trees of  ENTC, Department of Cibil Engineering and Department of Architecture.</t>
+  </si>
+  <si>
+    <t>Observed in Kaju kele area and at the boat yard.</t>
+  </si>
+  <si>
+    <t>Observed in the university ground premises.</t>
+  </si>
+  <si>
+    <t>Fairly common to see in university ground premises.</t>
+  </si>
+  <si>
+    <t>Observed around the Faculty of IT. Fairly Common in Kaju kele and Area around the Boat yard.</t>
+  </si>
+  <si>
+    <t>Many areas including the surrounding area of Department of FD &amp; PD. Also observed in the trees around the Bhavana and Trees of Ceremonial courtyard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many areas including the Kaju Kele area, Also observed in the trees around the Bhavana and Trees of Ceremonial courtyard. </t>
+  </si>
+  <si>
+    <t>Faily common to see inside Kaju kele. Also can be seen on the tree tops of edges of the university ground premises, Lagan and the Library.</t>
+  </si>
+  <si>
+    <t>Kaju kele,Boat yard, wooded areas around the department of Architecture, and Lagan.</t>
+  </si>
+  <si>
+    <t>Can be seen in flight at evenings/mornings above the university ground premises. Also very common inside Kaju kele.</t>
+  </si>
+  <si>
+    <t>Very common to see throughout the university.</t>
+  </si>
+  <si>
+    <t>Boart yard and the surrounding shallow areas of Bolgoda lake.</t>
+  </si>
+  <si>
+    <t>Can be observed in seetha gangula area at night. One specimen was recorded trapped inside a building during day time.</t>
+  </si>
+  <si>
+    <t>Can be seen throughout the university including inside the goda and goda uda canteen buildings. Very common in Kaju kele area.</t>
+  </si>
+  <si>
+    <t>BROWN SHRIKE</t>
+  </si>
+  <si>
+    <t>SRI LANKA GREEN PIGEON</t>
+  </si>
+  <si>
+    <t>WHITE-RUMPED MUNIA</t>
+  </si>
+  <si>
+    <t>LITTLE TERN</t>
+  </si>
+  <si>
+    <t>ASIAN BROWN FLYCATCHER</t>
+  </si>
+  <si>
+    <t>INDIAN WHITE-EYE</t>
+  </si>
+  <si>
+    <t>CHANGEABLE-HAWK EAGLE</t>
+  </si>
+  <si>
+    <t>CRESTED SERPENT EAGLE</t>
+  </si>
+  <si>
+    <t>STIATED HERON</t>
+  </si>
+  <si>
+    <t>BLACK-WINGED STILT</t>
+  </si>
+  <si>
+    <t>Pericrocotus cinnamomeus</t>
+  </si>
+  <si>
+    <t>SMALL MINIVET</t>
+  </si>
+  <si>
+    <t>Campephagidae</t>
+  </si>
+  <si>
+    <t>Lanius cristatus</t>
+  </si>
+  <si>
+    <t>Laniidae</t>
+  </si>
+  <si>
+    <t>Treron pompadora</t>
+  </si>
+  <si>
+    <t>Lonchura striata</t>
+  </si>
+  <si>
+    <t>JERDON'S LEAFBIRD</t>
+  </si>
+  <si>
+    <t>Chloropsis jerdoni</t>
+  </si>
+  <si>
+    <t>Chloropseidae</t>
+  </si>
+  <si>
+    <t>Sternula albifrons</t>
+  </si>
+  <si>
+    <t>Muscicapa dauurica</t>
+  </si>
+  <si>
+    <t>Zosterops palpebrosus</t>
+  </si>
+  <si>
+    <t>Oriental White-Eye</t>
+  </si>
+  <si>
+    <t>Zosteropidae</t>
+  </si>
+  <si>
+    <t>Crested Hawk-eagle</t>
+  </si>
+  <si>
+    <t>Nisaetus cirrhatus</t>
+  </si>
+  <si>
+    <t>Accipitridae</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spilornis cheela</t>
+  </si>
+  <si>
+    <t>Butorides striata</t>
+  </si>
+  <si>
+    <t>Green-Backed Heron</t>
+  </si>
+  <si>
+    <t>Himantopus himantopus</t>
+  </si>
+  <si>
+    <t>Recurvirostridae</t>
   </si>
 </sst>
 </file>
@@ -1417,12 +1543,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1433,8 +1553,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1472,11 +1598,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1509,19 +1646,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1742,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1761,7 +1901,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1807,17 +1947,17 @@
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>394</v>
+      <c r="D2" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>439</v>
+        <v>413</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>12</v>
@@ -1853,29 +1993,29 @@
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>394</v>
+      <c r="D3" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1897,29 +2037,29 @@
     </row>
     <row r="4" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>393</v>
+      <c r="D4" s="25" t="s">
+        <v>369</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1941,31 +2081,31 @@
     </row>
     <row r="5" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>29</v>
+        <v>384</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>394</v>
+      <c r="D5" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>438</v>
+        <v>412</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1987,29 +2127,29 @@
     </row>
     <row r="6" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>34</v>
+        <v>385</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>394</v>
+        <v>33</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -2031,31 +2171,31 @@
     </row>
     <row r="7" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="B7" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2077,28 +2217,28 @@
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>413</v>
-      </c>
-      <c r="B8" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2120,31 +2260,31 @@
     </row>
     <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="F9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2166,31 +2306,31 @@
     </row>
     <row r="10" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="D10" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="F10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="I10" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2212,29 +2352,29 @@
     </row>
     <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>394</v>
+      <c r="D11" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -2256,29 +2396,29 @@
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>394</v>
+      <c r="D12" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="I12" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2300,31 +2440,31 @@
     </row>
     <row r="13" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="F13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2346,31 +2486,31 @@
     </row>
     <row r="14" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="D14" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="F14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2392,29 +2532,29 @@
     </row>
     <row r="15" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>394</v>
+        <v>79</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -2436,31 +2576,31 @@
     </row>
     <row r="16" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="F16" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="I16" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -2482,31 +2622,31 @@
     </row>
     <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="B17" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="I17" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2528,29 +2668,29 @@
     </row>
     <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>394</v>
+        <v>79</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>36</v>
+        <v>421</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2572,29 +2712,29 @@
     </row>
     <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>108</v>
+        <v>389</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>105</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>394</v>
+        <v>106</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
-        <v>110</v>
+        <v>422</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2616,29 +2756,29 @@
     </row>
     <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>394</v>
+        <v>112</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>36</v>
+        <v>423</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2660,29 +2800,29 @@
     </row>
     <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>121</v>
+        <v>116</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>117</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>394</v>
+        <v>112</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>36</v>
+        <v>424</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2704,29 +2844,29 @@
     </row>
     <row r="22" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>122</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>394</v>
+        <v>123</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="6" t="s">
-        <v>128</v>
+        <v>425</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2748,31 +2888,31 @@
     </row>
     <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="H23" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>395</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -2794,29 +2934,29 @@
     </row>
     <row r="24" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>141</v>
+        <v>135</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>136</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>394</v>
+        <v>129</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -2838,31 +2978,31 @@
     </row>
     <row r="25" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>396</v>
+        <v>141</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>372</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>394</v>
+        <v>129</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>148</v>
+        <v>426</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -2884,31 +3024,31 @@
     </row>
     <row r="26" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I26" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -2930,31 +3070,31 @@
     </row>
     <row r="27" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>160</v>
+        <v>153</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>394</v>
+        <v>148</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>155</v>
+        <v>427</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -2976,31 +3116,31 @@
     </row>
     <row r="28" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>166</v>
+        <v>159</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>160</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>397</v>
+        <v>161</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>373</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>168</v>
+        <v>428</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -3022,31 +3162,31 @@
     </row>
     <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>173</v>
+        <v>165</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>166</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="F29" s="6" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -3068,31 +3208,31 @@
     </row>
     <row r="30" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>179</v>
+        <v>390</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>394</v>
+        <v>173</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -3114,29 +3254,29 @@
     </row>
     <row r="31" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>417</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>186</v>
+        <v>391</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>179</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>394</v>
+        <v>180</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="16" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3158,31 +3298,31 @@
     </row>
     <row r="32" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>418</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>192</v>
+        <v>392</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>185</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>394</v>
+        <v>186</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>434</v>
+        <v>408</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>194</v>
+        <v>429</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3204,29 +3344,29 @@
     </row>
     <row r="33" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>191</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>407</v>
+        <v>192</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>383</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="16" t="s">
-        <v>201</v>
+        <v>430</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3248,29 +3388,29 @@
     </row>
     <row r="34" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>206</v>
+        <v>196</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>197</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>394</v>
+        <v>192</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="6" t="s">
-        <v>207</v>
+        <v>431</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3292,29 +3432,29 @@
     </row>
     <row r="35" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>419</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>211</v>
+        <v>393</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>394</v>
+        <v>202</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
-        <v>36</v>
+        <v>420</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3336,29 +3476,29 @@
     </row>
     <row r="36" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>217</v>
+        <v>206</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>207</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>407</v>
+        <v>208</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>383</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="6" t="s">
-        <v>36</v>
+        <v>420</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -3380,29 +3520,29 @@
     </row>
     <row r="37" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>420</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>398</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="D37" s="26" t="s">
         <v>394</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="6" t="s">
-        <v>223</v>
+        <v>432</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3424,29 +3564,29 @@
     </row>
     <row r="38" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>399</v>
+        <v>395</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>375</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>394</v>
+        <v>216</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="6" t="s">
-        <v>228</v>
+        <v>433</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -3468,31 +3608,31 @@
     </row>
     <row r="39" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>400</v>
+        <v>220</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>376</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>394</v>
+        <v>216</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>433</v>
+        <v>407</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>233</v>
+        <v>434</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3514,29 +3654,29 @@
     </row>
     <row r="40" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>237</v>
+        <v>396</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>224</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>395</v>
+        <v>225</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>371</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6" t="s">
-        <v>239</v>
+        <v>435</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -3558,29 +3698,29 @@
     </row>
     <row r="41" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>244</v>
+        <v>229</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>230</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>394</v>
+        <v>231</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6" t="s">
-        <v>246</v>
+        <v>436</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3602,29 +3742,29 @@
     </row>
     <row r="42" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="B42" s="30" t="s">
-        <v>401</v>
+        <v>235</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>377</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>407</v>
+        <v>236</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>383</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>252</v>
+        <v>437</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3646,29 +3786,29 @@
     </row>
     <row r="43" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>257</v>
+        <v>240</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>241</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>394</v>
+        <v>236</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="6" t="s">
-        <v>258</v>
+        <v>438</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3690,29 +3830,29 @@
     </row>
     <row r="44" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="B44" s="27" t="s">
-        <v>263</v>
+        <v>245</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>246</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>394</v>
+        <v>247</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="19" t="s">
-        <v>409</v>
+      <c r="F44" s="30" t="s">
+        <v>439</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -3734,31 +3874,31 @@
     </row>
     <row r="45" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>268</v>
+        <v>397</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>251</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>407</v>
+        <v>247</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>383</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -3780,29 +3920,29 @@
     </row>
     <row r="46" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>402</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>403</v>
+        <v>378</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>379</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>394</v>
+        <v>247</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -3824,29 +3964,29 @@
     </row>
     <row r="47" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>424</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>278</v>
+        <v>398</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>261</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="D47" s="26" t="s">
-        <v>394</v>
+        <v>262</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6" t="s">
-        <v>280</v>
+        <v>441</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -3868,31 +4008,31 @@
     </row>
     <row r="48" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>285</v>
+        <v>266</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>267</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>394</v>
+        <v>262</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>280</v>
+        <v>440</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -3914,29 +4054,29 @@
     </row>
     <row r="49" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>290</v>
+        <v>271</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>272</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>407</v>
+        <v>273</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>383</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -3958,29 +4098,29 @@
     </row>
     <row r="50" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>294</v>
+        <v>399</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>276</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D50" s="26" t="s">
-        <v>394</v>
+        <v>273</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>370</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="6" t="s">
-        <v>295</v>
+        <v>442</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -4002,29 +4142,29 @@
     </row>
     <row r="51" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>298</v>
+        <v>400</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>279</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>394</v>
+        <v>280</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="6" t="s">
-        <v>36</v>
+        <v>421</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4046,31 +4186,31 @@
     </row>
     <row r="52" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>304</v>
+        <v>284</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>285</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>394</v>
+        <v>286</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -4092,29 +4232,29 @@
     </row>
     <row r="53" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>311</v>
+        <v>291</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>292</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>404</v>
+        <v>286</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>380</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4136,29 +4276,29 @@
     </row>
     <row r="54" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>316</v>
+        <v>296</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>297</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>394</v>
+        <v>286</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -4180,31 +4320,31 @@
     </row>
     <row r="55" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="B55" s="23" t="s">
-        <v>320</v>
+        <v>300</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>301</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>394</v>
+        <v>302</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>323</v>
+        <v>443</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4226,29 +4366,29 @@
     </row>
     <row r="56" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="B56" s="23" t="s">
-        <v>328</v>
+        <v>307</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>308</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>405</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>394</v>
+        <v>381</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="6" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -4270,31 +4410,31 @@
     </row>
     <row r="57" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>333</v>
+        <v>401</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>313</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>394</v>
+        <v>381</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>335</v>
+        <v>444</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4316,29 +4456,29 @@
     </row>
     <row r="58" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>339</v>
+        <v>402</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>394</v>
+        <v>319</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="6" t="s">
-        <v>341</v>
+        <v>445</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>342</v>
+        <v>320</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4360,29 +4500,29 @@
     </row>
     <row r="59" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="B59" s="20" t="s">
-        <v>345</v>
+        <v>403</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>323</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>394</v>
+        <v>319</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -4404,29 +4544,29 @@
     </row>
     <row r="60" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="B60" s="21" t="s">
-        <v>350</v>
+        <v>404</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>328</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>394</v>
+        <v>329</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="6" t="s">
-        <v>352</v>
+        <v>446</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -4448,29 +4588,29 @@
     </row>
     <row r="61" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B61" s="21" t="s">
-        <v>406</v>
+        <v>334</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>382</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>394</v>
+        <v>329</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="6" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -4492,31 +4632,31 @@
     </row>
     <row r="62" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B62" s="21" t="s">
-        <v>361</v>
+        <v>338</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>339</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>404</v>
+        <v>340</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>380</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>367</v>
+        <v>345</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -4538,31 +4678,31 @@
     </row>
     <row r="63" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="B63" s="21" t="s">
-        <v>369</v>
+        <v>346</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>347</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>394</v>
+        <v>340</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>432</v>
+        <v>406</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>370</v>
+        <v>447</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -4584,31 +4724,31 @@
     </row>
     <row r="64" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B64" s="21" t="s">
-        <v>375</v>
+        <v>351</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>352</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>394</v>
+        <v>353</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>378</v>
+        <v>448</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -4630,31 +4770,31 @@
     </row>
     <row r="65" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="B65" s="21" t="s">
-        <v>382</v>
+        <v>405</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>358</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>394</v>
+        <v>359</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>36</v>
+        <v>417</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -4674,7 +4814,19 @@
       <c r="Y65" s="4"/>
       <c r="Z65" s="4"/>
     </row>
-    <row r="66" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="31" t="s">
+        <v>460</v>
+      </c>
+      <c r="B66" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="C66" t="s">
+        <v>461</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -4699,10 +4851,18 @@
       <c r="Z66" s="4"/>
     </row>
     <row r="67" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
+      <c r="A67" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="B67" s="33" t="s">
+        <v>462</v>
+      </c>
+      <c r="C67" t="s">
+        <v>463</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>383</v>
+      </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -4727,10 +4887,18 @@
       <c r="Z67" s="4"/>
     </row>
     <row r="68" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
+      <c r="A68" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="C68" t="s">
+        <v>129</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -4755,10 +4923,18 @@
       <c r="Z68" s="4"/>
     </row>
     <row r="69" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
+      <c r="A69" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B69" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="C69" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -4783,10 +4959,18 @@
       <c r="Z69" s="4"/>
     </row>
     <row r="70" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
+      <c r="A70" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B70" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="C70" t="s">
+        <v>468</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -4811,10 +4995,18 @@
       <c r="Z70" s="4"/>
     </row>
     <row r="71" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
+      <c r="A71" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B71" s="32" t="s">
+        <v>469</v>
+      </c>
+      <c r="C71" t="s">
+        <v>208</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>369</v>
+      </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -4839,10 +5031,18 @@
       <c r="Z71" s="4"/>
     </row>
     <row r="72" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
+      <c r="A72" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="B72" s="33" t="s">
+        <v>470</v>
+      </c>
+      <c r="C72" t="s">
+        <v>247</v>
+      </c>
+      <c r="D72" s="28" t="s">
+        <v>383</v>
+      </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -4867,11 +5067,21 @@
       <c r="Z72" s="4"/>
     </row>
     <row r="73" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
+      <c r="A73" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B73" s="32" t="s">
+        <v>471</v>
+      </c>
+      <c r="C73" t="s">
+        <v>473</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>472</v>
+      </c>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
@@ -4895,11 +5105,21 @@
       <c r="Z73" s="4"/>
     </row>
     <row r="74" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
+      <c r="A74" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B74" s="32" t="s">
+        <v>475</v>
+      </c>
+      <c r="C74" t="s">
+        <v>476</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="E74" t="s">
+        <v>474</v>
+      </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -4923,10 +5143,18 @@
       <c r="Z74" s="4"/>
     </row>
     <row r="75" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
+      <c r="A75" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="B75" s="32" t="s">
+        <v>477</v>
+      </c>
+      <c r="C75" t="s">
+        <v>476</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -4951,11 +5179,21 @@
       <c r="Z75" s="4"/>
     </row>
     <row r="76" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
+      <c r="A76" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="B76" s="32" t="s">
+        <v>478</v>
+      </c>
+      <c r="C76" t="s">
+        <v>79</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>479</v>
+      </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
@@ -4979,10 +5217,18 @@
       <c r="Z76" s="4"/>
     </row>
     <row r="77" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
+      <c r="A77" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="B77" s="32" t="s">
+        <v>480</v>
+      </c>
+      <c r="C77" t="s">
+        <v>481</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>

</xml_diff>

<commit_message>
closes #6 and #8
</commit_message>
<xml_diff>
--- a/uomBirds.xlsx
+++ b/uomBirds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1FCA6B-1302-42F9-A407-701BC29D7C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8E277C-80B1-4B54-B4E3-EE846166CAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="530">
   <si>
     <t>Common Name</t>
   </si>
@@ -1502,6 +1502,114 @@
   </si>
   <si>
     <t>Observed only once at Boat yard in flight.</t>
+  </si>
+  <si>
+    <t>The shrike displays predominantly brown plumage on its upper body, featuring a rounded tail. In winter, the black mask may appear lighter, accompanied by a white brow above it. Its underparts are creamy with rufous flanks and belly, while the wings are brown without any distinctive white "mirror" patches. Female shrikes typically exhibit subtle scalloping on the underside, and their dark brown masks are less pronounced compared to males.</t>
+  </si>
+  <si>
+    <t>A medium-sized green pigeon with a distinctive yellow face and a yellowish line along the wing is observed. In the male, the back is maroon, transitioning to green in the female.</t>
+  </si>
+  <si>
+    <t>This bird features a blackish-brown head and back, complemented by pure white underparts and rump. The back is finely streaked with pale shafts. Juveniles exhibit a rufous-brown hue with indistinct streaks above, a buffy gray rump, light rufous breast, and buffy gray underparts. Variations among races are notable in terms of the quantity of white-and-gray streaking on the underparts and the extent of blackish-brown coloring on the head.</t>
+  </si>
+  <si>
+    <t>This vibrant bird, residing in lush green forests, displays a crisp emerald-green plumage. The male is characterized by a dark blue throat patch bordered by a thick black outline, while the female exhibits a pale blue throat without the dark border. In its range, the Golden-fronted Leafbird is the only similarly-colored bird, easily distinguishable by its orange forehead.</t>
+  </si>
+  <si>
+    <t>This diminutive tern has a delicate appearance, with distinctive features in its breeding plumage. It sports a black cap accompanied by a white forehead chevron and a black-tipped yellow bill. Its small size makes it easily recognizable. Keep an eye out for black stripes extending from the shoulder to the wingtip as a key identifying characteristic.</t>
+  </si>
+  <si>
+    <t>This unadorned brown flycatcher possesses a notably large-eyed appearance. Its distinguishing features include a bright white eyering and unmarked throat and underparts. When compared to other similar brownish flycatchers, it appears shorter- and plainer-winged.</t>
+  </si>
+  <si>
+    <t>yellowish olive upper parts, a white eye ring, yellow throat and, a vent. The belly is whitish grey but may have yellow in some subspecies. The sexes look similar.</t>
+  </si>
+  <si>
+    <t>This medium-sized eagle boasts massive rounded wings and is characterized by two primary color morphs: pale and black. In the pale morph, adults display dark brown upperparts with a white breast marked by dark streaks, while juveniles exhibit a much paler plumage with cleaner white underparts and less extensive striping and barring throughout the body. The dark morph is uniformly dark with slightly paler outer wing feathers, posing a potential resemblance to dark Honey-Buzzards. However, distinguishing features include the hawk-eagle's longer wings and more slender profile.</t>
+  </si>
+  <si>
+    <t>A rather large, heavily built eagle with a dark, white-tipped bushy crest that gives it a distinctive large-headed look. When raised in alarm, the crest frames the whole face, highlighting the bare yellow lores and eyes, making the head look larger and fiercer. The rufous-brown underparts have neatly arranged dark-edged bold white spots. In flight, shows broad rounded wings with a wide black trailing edge. Juvenile predominantly white with dark streaks below; also note dark mask.</t>
+  </si>
+  <si>
+    <t>Distinguished by its small size and predominantly gray plumage, this bird stands apart from most other herons and bitterns. Key identifying features include a contrasting dark cap, well-defined pale edges on wing feathers, and distinct white and rufous stripes on the front of the neck. Juveniles exhibit a streakier pattern below compared to adults, with a mostly gray neck featuring restricted rufous coloring.</t>
+  </si>
+  <si>
+    <t>These adult birds are characterized by their lengthy build, featuring long pink legs and a slender black bill. Typically, their plumage is black above and white below, accompanied by a white head and neck. The amount of black on the head and neck varies depending on the species. Male individuals often display a black back with a greenish gloss or sheen, while females have a brownish hue on their backs, creating a noticeable contrast with the black remiges.</t>
+  </si>
+  <si>
+    <t>The Small Minivet sustains itself primarily on an insect-based diet, which includes caterpillars, beetles, bugs, and ants. These agile hunters showcase their ability to catch prey mid-air or skillfully pluck insects from leaves while perched.</t>
+  </si>
+  <si>
+    <t>The Small Minivet is characterized by a robust dark beak and elongated wings. Distinguishing itself from other typical minivets, the male exhibits grey upperparts and head instead of glossy black. Its underparts are adorned in orange, transitioning to yellow on the belly, complemented by orange tail edges, rump, and wing patches. Conversely, the female presents a grey upper body with yellow underparts, including the face. Similar to the male, she features yellow tail edges, rump, and wing patches.</t>
+  </si>
+  <si>
+    <t>The primary diet of this bird includes insects, as well as small birds and mammals. It employs a hunting technique commonly observed in shrikes, where it makes a quick sally from a prominent perch to catch its prey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eats the seeds and fruits of a wide variety of plants.</t>
+  </si>
+  <si>
+    <t>This sociable bird displays gregarious behavior and primarily sustains itself by consuming seeds. It can be observed moving in groups through the undergrowth while foraging.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This species eats insects, fruit and nectar. </t>
+  </si>
+  <si>
+    <t>These birds engage in feeding activities just offshore, in shallow waters along protected coastlines, where they consume a diet consisting of fish, crustaceans, and invertebrates. A distinctive foraging behavior observed in them is plunge-diving for fish along the shoreline. This feeding proximity to the shore distinguishes them from other seabirds, which may undertake long flights in search of food.</t>
+  </si>
+  <si>
+    <t>While primarily insectivorous, the Indian White-eye also incorporates nectar and various fruits into its diet.</t>
+  </si>
+  <si>
+    <t>The Asian Brown Flycatcher predominantly feeds on flying insects, employing a sallying technique where it launches from a perch to catch its prey in mid-air.</t>
+  </si>
+  <si>
+    <t>This predator has a diverse diet, preying on a variety of animals including mammals, large birds, reptiles such as snakes and lizards, fish and amphibians like frogs.</t>
+  </si>
+  <si>
+    <t>This species is primarily a snake-hunter, displaying a particular preference for tree snakes. However, its diet extends beyond serpents to include lizards, frogs, toads, mammals, eels, and small birds.</t>
+  </si>
+  <si>
+    <t>The Striated Heron primarily feeds on a diet consisting of crabs and other crustaceans. Additionally, it includes mollusks and small fish in its feeding repertoire.</t>
+  </si>
+  <si>
+    <t>Black-winged Stilts are carnivores. They use their sharp bills to peck and ingest only very small food such as molluscs, miniscule crustaceans, algae, flies and aquatic insects.</t>
+  </si>
+  <si>
+    <t>Uncommon breeding resident from lowlands up to mid hills. Open forests and bushes with scattered trees are the places to look for.</t>
+  </si>
+  <si>
+    <t>Common throughout the Island. Can be observed in open country with trees or bushes.</t>
+  </si>
+  <si>
+    <t>Farily common breeding resident in lowlands to lower hills. Local and uncommon up to mid hills. Preffered habitats are forests and woods.</t>
+  </si>
+  <si>
+    <t>Uncommon breeding resident from lowlands up to mid hills. More common to see in dry zone.Foresets,wooded areas and gardens are the preffered habitats.</t>
+  </si>
+  <si>
+    <t>Fairly common breeding resident in lowlands up to mid hills.Preffered habitats include forests, Open wooded areas, scrub and cultivation.</t>
+  </si>
+  <si>
+    <t>Farily common and local breeding resident in dry zone and visitor to the wet zone. Can be seen in coastal wetlands and inland tanks.</t>
+  </si>
+  <si>
+    <t>Fairly common winter migrant in lowlands up to mid hills. Open wooded areas, plantations and garden are the preffered habitat.</t>
+  </si>
+  <si>
+    <t>Farily common breeding resident from lowlands upto mid hills. Uncommon in high hills. Can be seen around trees.</t>
+  </si>
+  <si>
+    <t>Fairly common locally througout the Isand and and a breeding resident. Well wooded areas is the preffered habitat.</t>
+  </si>
+  <si>
+    <t>Fairly common breeding resident which is found thougout Sri Lanka. Can be seen in forests and wooded areas.</t>
+  </si>
+  <si>
+    <t>Fairly uncommon breeding resident in lowlands and lower hills. Mangroves and dense vegetations at the edges of the rivers, marshes and tanks, open edges of lagoons are the preffered habitats.</t>
+  </si>
+  <si>
+    <t>In dry lowlands, a fairly common breeding resident. A few birds breed in wet lowlands others are winter migrants in the lowlands. Freshwater and brackish shallow waters in marshes, lagoons and tanks are the preffered habitats.</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1668,17 +1776,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1695,9 +1795,22 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1918,8 +2031,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1937,7 +2050,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1983,13 +2096,13 @@
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -2029,13 +2142,13 @@
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -2075,13 +2188,13 @@
       <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>369</v>
       </c>
       <c r="E4" s="4"/>
@@ -2119,13 +2232,13 @@
       <c r="A5" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -2161,31 +2274,33 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
     </row>
-    <row r="6" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="25" t="s">
+    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>475</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>476</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="8" t="s">
-        <v>417</v>
+      <c r="E6" s="33" t="s">
+        <v>474</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>489</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>526</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>36</v>
+        <v>501</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>37</v>
+        <v>514</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -2205,33 +2320,31 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="25" t="s">
+    <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>477</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>476</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>418</v>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>491</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>527</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>40</v>
+        <v>502</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>41</v>
+        <v>515</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2253,28 +2366,29 @@
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>45</v>
+      <c r="E8" s="34"/>
+      <c r="F8" s="36" t="s">
+        <v>417</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>37</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2294,33 +2408,33 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>47</v>
+    <row r="9" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>34</v>
+        <v>411</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>418</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>364</v>
+        <v>41</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2342,31 +2456,29 @@
     </row>
     <row r="10" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>52</v>
+        <v>387</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="33"/>
+      <c r="F10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>55</v>
+      <c r="G10" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2387,30 +2499,32 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>59</v>
+      <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>63</v>
+        <v>364</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -2432,29 +2546,31 @@
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>65</v>
+        <v>51</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F12" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2474,33 +2590,31 @@
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>72</v>
+    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>67</v>
+        <v>60</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2522,31 +2636,29 @@
     </row>
     <row r="14" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>78</v>
+        <v>64</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="6" t="s">
-        <v>34</v>
+        <v>419</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2568,29 +2680,31 @@
     </row>
     <row r="15" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>85</v>
+        <v>71</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>72</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="F15" s="8" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -2612,31 +2726,31 @@
     </row>
     <row r="16" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>90</v>
+        <v>77</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>420</v>
+        <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -2658,31 +2772,29 @@
     </row>
     <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>95</v>
+        <v>84</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>96</v>
+      <c r="E17" s="4"/>
+      <c r="F17" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2702,31 +2814,33 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>101</v>
+    <row r="18" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>90</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
-        <v>421</v>
+      <c r="E18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>420</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -2748,29 +2862,31 @@
     </row>
     <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>105</v>
+        <v>388</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>95</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>410</v>
+      </c>
       <c r="F19" s="6" t="s">
-        <v>422</v>
+        <v>96</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2791,30 +2907,30 @@
       <c r="Z19" s="4"/>
     </row>
     <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>111</v>
+      <c r="A20" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2835,30 +2951,32 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="25" t="s">
+      <c r="A21" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>478</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>479</v>
+      </c>
       <c r="F21" s="4" t="s">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>118</v>
+        <v>528</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>119</v>
+        <v>503</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>120</v>
+        <v>516</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2880,29 +2998,31 @@
     </row>
     <row r="22" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="25" t="s">
+        <v>460</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>459</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>461</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6" t="s">
-        <v>425</v>
+      <c r="E22" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>482</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>124</v>
+        <v>518</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>125</v>
+        <v>506</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>126</v>
+        <v>505</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2923,32 +3043,30 @@
       <c r="Z22" s="4"/>
     </row>
     <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>128</v>
+      <c r="A23" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>105</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>371</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>130</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="6" t="s">
-        <v>131</v>
+        <v>422</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -2968,31 +3086,31 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
     </row>
-    <row r="24" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="25" t="s">
+    <row r="24" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>468</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="6" t="s">
-        <v>137</v>
+      <c r="F24" s="4" t="s">
+        <v>487</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>138</v>
+        <v>521</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>139</v>
+        <v>497</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>140</v>
+        <v>510</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -3012,33 +3130,31 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
     </row>
-    <row r="25" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>372</v>
+    <row r="25" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>111</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>426</v>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>423</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -3058,33 +3174,31 @@
       <c r="Y25" s="4"/>
       <c r="Z25" s="4"/>
     </row>
-    <row r="26" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>147</v>
+    <row r="26" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>117</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D26" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>149</v>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>424</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -3106,31 +3220,29 @@
     </row>
     <row r="27" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>154</v>
+        <v>121</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>122</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3151,32 +3263,32 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>160</v>
+      <c r="A28" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>373</v>
+        <v>129</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>428</v>
+        <v>131</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -3198,31 +3310,29 @@
     </row>
     <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>166</v>
+        <v>135</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>167</v>
-      </c>
+      <c r="E29" s="4"/>
       <c r="F29" s="6" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -3244,31 +3354,31 @@
     </row>
     <row r="30" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>390</v>
+        <v>141</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>172</v>
+        <v>372</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D30" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>175</v>
+        <v>426</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -3288,31 +3398,31 @@
       <c r="Y30" s="4"/>
       <c r="Z30" s="4"/>
     </row>
-    <row r="31" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>391</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D31" s="25" t="s">
+    <row r="31" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="16" t="s">
-        <v>181</v>
+      <c r="F31" s="34" t="s">
+        <v>485</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>182</v>
+        <v>520</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>183</v>
+        <v>495</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>184</v>
+        <v>508</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -3332,33 +3442,33 @@
       <c r="Y31" s="4"/>
       <c r="Z31" s="4"/>
     </row>
-    <row r="32" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>185</v>
+    <row r="32" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D32" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>429</v>
+        <v>409</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>149</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3380,29 +3490,31 @@
     </row>
     <row r="33" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>191</v>
+        <v>153</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>154</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D33" s="28" t="s">
-        <v>383</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="16" t="s">
-        <v>430</v>
+        <v>148</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>427</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3423,30 +3535,32 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="D34" s="25" t="s">
+      <c r="A34" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="20" t="s">
+        <v>373</v>
+      </c>
       <c r="F34" s="6" t="s">
-        <v>431</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>200</v>
+        <v>428</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3466,31 +3580,33 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
     </row>
-    <row r="35" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>201</v>
+    <row r="35" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>166</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D35" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4" t="s">
-        <v>420</v>
+      <c r="E35" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3512,29 +3628,31 @@
     </row>
     <row r="36" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>207</v>
+        <v>390</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>172</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>383</v>
-      </c>
-      <c r="E36" s="4"/>
+        <v>173</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="F36" s="6" t="s">
-        <v>420</v>
+        <v>175</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -3556,29 +3674,29 @@
     </row>
     <row r="37" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>394</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>374</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="D37" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D37" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="6" t="s">
-        <v>432</v>
+        <v>181</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3598,31 +3716,33 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
     </row>
-    <row r="38" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>375</v>
+    <row r="38" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="D38" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="6" t="s">
-        <v>433</v>
+      <c r="E38" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>429</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -3642,33 +3762,31 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
     </row>
-    <row r="39" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>376</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="D39" s="25" t="s">
+    <row r="39" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>407</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>223</v>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>509</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3690,29 +3808,29 @@
     </row>
     <row r="40" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>224</v>
+        <v>190</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>191</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>371</v>
+        <v>192</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>383</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -3733,30 +3851,30 @@
       <c r="Z40" s="4"/>
     </row>
     <row r="41" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D41" s="25" t="s">
+      <c r="A41" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D41" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="13"/>
       <c r="F41" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>234</v>
+        <v>431</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3776,31 +3894,31 @@
       <c r="Y41" s="4"/>
       <c r="Z41" s="4"/>
     </row>
-    <row r="42" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>377</v>
+    <row r="42" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>201</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>383</v>
+        <v>202</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>370</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="6" t="s">
-        <v>437</v>
+      <c r="F42" s="4" t="s">
+        <v>420</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3820,31 +3938,31 @@
       <c r="Y42" s="4"/>
       <c r="Z42" s="4"/>
     </row>
-    <row r="43" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>370</v>
+    <row r="43" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>462</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>463</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>383</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="6" t="s">
-        <v>438</v>
+      <c r="F43" s="4" t="s">
+        <v>484</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>242</v>
+        <v>519</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>243</v>
+        <v>494</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>244</v>
+        <v>507</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3866,29 +3984,29 @@
     </row>
     <row r="44" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>246</v>
+        <v>206</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>207</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>370</v>
+        <v>208</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>383</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="30" t="s">
-        <v>439</v>
+      <c r="F44" s="6" t="s">
+        <v>420</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>248</v>
+        <v>209</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>249</v>
+        <v>210</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>250</v>
+        <v>211</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -3908,33 +4026,31 @@
       <c r="Y44" s="4"/>
       <c r="Z44" s="4"/>
     </row>
-    <row r="45" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
-        <v>397</v>
+    <row r="45" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>452</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>383</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>253</v>
+        <v>469</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>420</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>254</v>
+        <v>523</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>255</v>
+        <v>498</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>256</v>
+        <v>511</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -3954,31 +4070,31 @@
       <c r="Y45" s="4"/>
       <c r="Z45" s="4"/>
     </row>
-    <row r="46" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>378</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>379</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D46" s="25" t="s">
+    <row r="46" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>257</v>
+      <c r="F46" s="6" t="s">
+        <v>432</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -4000,29 +4116,29 @@
     </row>
     <row r="47" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>261</v>
+        <v>375</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D47" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D47" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>263</v>
+        <v>217</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>264</v>
+        <v>218</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>265</v>
+        <v>219</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -4043,32 +4159,32 @@
       <c r="Z47" s="4"/>
     </row>
     <row r="48" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>266</v>
+      <c r="A48" s="14" t="s">
+        <v>220</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D48" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>268</v>
+      <c r="E48" s="13" t="s">
+        <v>407</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>365</v>
+        <v>434</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>223</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -4089,30 +4205,30 @@
       <c r="Z48" s="4"/>
     </row>
     <row r="49" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="B49" s="27" t="s">
-        <v>272</v>
+      <c r="A49" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>224</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D49" s="28" t="s">
-        <v>383</v>
+        <v>225</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>371</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6" t="s">
-        <v>414</v>
+        <v>435</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>274</v>
+        <v>226</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>275</v>
+        <v>227</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>367</v>
+        <v>228</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -4134,29 +4250,29 @@
     </row>
     <row r="50" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>276</v>
+        <v>229</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>230</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D50" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="D50" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="6" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>366</v>
+        <v>234</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -4176,31 +4292,31 @@
       <c r="Y50" s="4"/>
       <c r="Z50" s="4"/>
     </row>
-    <row r="51" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>400</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>279</v>
+        <v>235</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>377</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>370</v>
+        <v>236</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>383</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="6" t="s">
-        <v>421</v>
+        <v>437</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>281</v>
+        <v>237</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>282</v>
+        <v>238</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4220,33 +4336,31 @@
       <c r="Y51" s="4"/>
       <c r="Z51" s="4"/>
     </row>
-    <row r="52" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>285</v>
+    <row r="52" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>241</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D52" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="D52" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>287</v>
-      </c>
+      <c r="E52" s="4"/>
       <c r="F52" s="6" t="s">
-        <v>34</v>
+        <v>438</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>288</v>
+        <v>242</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>289</v>
+        <v>243</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>290</v>
+        <v>244</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -4266,31 +4380,31 @@
       <c r="Y52" s="4"/>
       <c r="Z52" s="4"/>
     </row>
-    <row r="53" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>292</v>
+    <row r="53" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>246</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>380</v>
+        <v>247</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>370</v>
       </c>
       <c r="E53" s="4"/>
-      <c r="F53" s="6" t="s">
-        <v>34</v>
+      <c r="F53" s="26" t="s">
+        <v>439</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>294</v>
+        <v>249</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>295</v>
+        <v>250</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4310,31 +4424,33 @@
       <c r="Y53" s="4"/>
       <c r="Z53" s="4"/>
     </row>
-    <row r="54" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>296</v>
+        <v>397</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>297</v>
+        <v>251</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>370</v>
-      </c>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4" t="s">
-        <v>34</v>
+        <v>247</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>298</v>
+        <v>254</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>299</v>
+        <v>255</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>368</v>
+        <v>256</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -4354,33 +4470,31 @@
       <c r="Y54" s="4"/>
       <c r="Z54" s="4"/>
     </row>
-    <row r="55" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="D55" s="19" t="s">
+    <row r="55" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E55" s="17" t="s">
-        <v>303</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="H55" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="I55" s="17" t="s">
-        <v>306</v>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4400,31 +4514,31 @@
       <c r="Y55" s="4"/>
       <c r="Z55" s="4"/>
     </row>
-    <row r="56" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="B56" s="22" t="s">
-        <v>308</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>370</v>
-      </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>310</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>312</v>
+    <row r="56" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>513</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -4446,31 +4560,29 @@
     </row>
     <row r="57" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B57" s="20" t="s">
-        <v>313</v>
+        <v>398</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>261</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="D57" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D57" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>314</v>
-      </c>
+      <c r="E57" s="4"/>
       <c r="F57" s="6" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>315</v>
+        <v>263</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>316</v>
+        <v>264</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>317</v>
+        <v>265</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4492,29 +4604,31 @@
     </row>
     <row r="58" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>318</v>
+        <v>266</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>267</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="D58" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>370</v>
       </c>
-      <c r="E58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>268</v>
+      </c>
       <c r="F58" s="6" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>320</v>
+        <v>269</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>322</v>
+        <v>365</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4534,31 +4648,31 @@
       <c r="Y58" s="4"/>
       <c r="Z58" s="4"/>
     </row>
-    <row r="59" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>323</v>
+    <row r="59" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>272</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>370</v>
+        <v>273</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>383</v>
       </c>
       <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>324</v>
+      <c r="F59" s="6" t="s">
+        <v>414</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>326</v>
+        <v>275</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>327</v>
+        <v>367</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -4580,29 +4694,29 @@
     </row>
     <row r="60" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>328</v>
+        <v>399</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>276</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D60" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D60" s="21" t="s">
         <v>370</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="6" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>331</v>
+        <v>277</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>332</v>
+        <v>278</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>333</v>
+        <v>366</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -4622,31 +4736,31 @@
       <c r="Y60" s="4"/>
       <c r="Z60" s="4"/>
     </row>
-    <row r="61" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="B61" s="20" t="s">
-        <v>382</v>
+    <row r="61" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>279</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D61" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="D61" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="6" t="s">
-        <v>330</v>
+        <v>421</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>335</v>
+        <v>281</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>336</v>
+        <v>282</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>337</v>
+        <v>283</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -4666,33 +4780,33 @@
       <c r="Y61" s="4"/>
       <c r="Z61" s="4"/>
     </row>
-    <row r="62" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>339</v>
+    <row r="62" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>285</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D62" s="19" t="s">
-        <v>380</v>
+        <v>286</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>370</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>341</v>
+        <v>287</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>342</v>
+        <v>34</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>343</v>
+        <v>288</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>344</v>
+        <v>289</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>345</v>
+        <v>290</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -4712,33 +4826,31 @@
       <c r="Y62" s="4"/>
       <c r="Z62" s="4"/>
     </row>
-    <row r="63" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="B63" s="20" t="s">
-        <v>347</v>
+    <row r="63" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A63" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>292</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>370</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>406</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="E63" s="4"/>
       <c r="F63" s="6" t="s">
-        <v>447</v>
+        <v>34</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>348</v>
+        <v>293</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="I63" s="10" t="s">
-        <v>350</v>
+        <v>294</v>
+      </c>
+      <c r="I63" s="34" t="s">
+        <v>295</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -4758,33 +4870,31 @@
       <c r="Y63" s="4"/>
       <c r="Z63" s="4"/>
     </row>
-    <row r="64" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>352</v>
+    <row r="64" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>297</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D64" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="D64" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>448</v>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>355</v>
+        <v>298</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>356</v>
+        <v>299</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -4805,32 +4915,32 @@
       <c r="Z64" s="4"/>
     </row>
     <row r="65" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="B65" s="20" t="s">
-        <v>358</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="D65" s="19" t="s">
+      <c r="A65" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D65" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>360</v>
+      <c r="E65" s="13" t="s">
+        <v>303</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="H65" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>363</v>
+        <v>443</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>306</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -4851,27 +4961,31 @@
       <c r="Z65" s="4"/>
     </row>
     <row r="66" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="31" t="s">
-        <v>460</v>
-      </c>
-      <c r="B66" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="C66" t="s">
-        <v>461</v>
-      </c>
-      <c r="D66" s="19" t="s">
+      <c r="A66" s="30" t="s">
+        <v>307</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>381</v>
+      </c>
+      <c r="D66" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>312</v>
+      </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
@@ -4890,26 +5004,34 @@
       <c r="Y66" s="4"/>
       <c r="Z66" s="4"/>
     </row>
-    <row r="67" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="B67" s="33" t="s">
-        <v>462</v>
-      </c>
-      <c r="C67" t="s">
-        <v>463</v>
-      </c>
-      <c r="D67" s="28" t="s">
-        <v>383</v>
-      </c>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
+    <row r="67" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>381</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>317</v>
+      </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
@@ -4928,26 +5050,32 @@
       <c r="Y67" s="4"/>
       <c r="Z67" s="4"/>
     </row>
-    <row r="68" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="B68" s="32" t="s">
-        <v>464</v>
-      </c>
-      <c r="C68" t="s">
-        <v>129</v>
-      </c>
-      <c r="D68" s="19" t="s">
+    <row r="68" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="D68" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E68" s="4"/>
-      <c r="F68" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
+      <c r="F68" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>322</v>
+      </c>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
@@ -4968,24 +5096,30 @@
     </row>
     <row r="69" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="B69" s="32" t="s">
-        <v>465</v>
-      </c>
-      <c r="C69" t="s">
-        <v>186</v>
-      </c>
-      <c r="D69" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="C69" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="D69" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
+        <v>324</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>327</v>
+      </c>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
@@ -5004,26 +5138,32 @@
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
     </row>
-    <row r="70" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="B70" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="C70" t="s">
-        <v>468</v>
-      </c>
-      <c r="D70" s="19" t="s">
+    <row r="70" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="C70" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E70" s="4"/>
-      <c r="F70" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
+      <c r="F70" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>333</v>
+      </c>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
@@ -5042,26 +5182,32 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row r="71" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="B71" s="32" t="s">
-        <v>469</v>
-      </c>
-      <c r="C71" t="s">
-        <v>208</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>369</v>
+    <row r="71" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="C71" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>370</v>
       </c>
       <c r="E71" s="4"/>
-      <c r="F71" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
+      <c r="F71" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>337</v>
+      </c>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
@@ -5082,24 +5228,30 @@
     </row>
     <row r="72" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="B72" s="33" t="s">
-        <v>470</v>
+        <v>458</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>480</v>
       </c>
       <c r="C72" t="s">
-        <v>247</v>
-      </c>
-      <c r="D72" s="28" t="s">
-        <v>383</v>
+        <v>481</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>370</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
+        <v>492</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>517</v>
+      </c>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
@@ -5118,28 +5270,34 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row r="73" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="B73" s="32" t="s">
-        <v>471</v>
-      </c>
-      <c r="C73" t="s">
-        <v>473</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>370</v>
+    <row r="73" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="C73" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>380</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
+        <v>341</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>345</v>
+      </c>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
@@ -5158,28 +5316,34 @@
       <c r="Y73" s="4"/>
       <c r="Z73" s="4"/>
     </row>
-    <row r="74" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="B74" s="32" t="s">
-        <v>475</v>
-      </c>
-      <c r="C74" t="s">
-        <v>476</v>
-      </c>
-      <c r="D74" s="19" t="s">
+    <row r="74" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="C74" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D74" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E74" t="s">
-        <v>474</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
+      <c r="E74" s="34" t="s">
+        <v>406</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
@@ -5198,26 +5362,34 @@
       <c r="Y74" s="4"/>
       <c r="Z74" s="4"/>
     </row>
-    <row r="75" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="B75" s="32" t="s">
-        <v>477</v>
-      </c>
-      <c r="C75" t="s">
-        <v>476</v>
-      </c>
-      <c r="D75" s="19" t="s">
+    <row r="75" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C75" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="D75" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
+      <c r="E75" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>357</v>
+      </c>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
@@ -5236,28 +5408,34 @@
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
     </row>
-    <row r="76" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="B76" s="32" t="s">
-        <v>478</v>
-      </c>
-      <c r="C76" t="s">
-        <v>79</v>
-      </c>
-      <c r="D76" s="19" t="s">
+    <row r="76" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="C76" s="34" t="s">
+        <v>359</v>
+      </c>
+      <c r="D76" s="15" t="s">
         <v>370</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
+        <v>360</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
@@ -5278,24 +5456,32 @@
     </row>
     <row r="77" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="B77" s="32" t="s">
-        <v>480</v>
+        <v>454</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>471</v>
       </c>
       <c r="C77" t="s">
-        <v>481</v>
-      </c>
-      <c r="D77" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="D77" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E77" s="4"/>
+      <c r="E77" s="4" t="s">
+        <v>472</v>
+      </c>
       <c r="F77" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
+        <v>490</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>512</v>
+      </c>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
@@ -31160,6 +31346,9 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I77">
+    <sortCondition ref="C1:C77"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. sites responsiveness issue solved. 2. fixes #10 . 3. Added link and a QR to the site in the latex doc. 4.Added a footnote for H:,D:,R:
</commit_message>
<xml_diff>
--- a/uomBirds.xlsx
+++ b/uomBirds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21B8F9E-EC1F-414C-B3ED-F893E11175C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8F854C-0F9F-404A-AD50-E1ED9A3C5E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1730,7 +1730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1796,6 +1796,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2016,9 +2017,9 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R74" sqref="R74"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4353,7 +4354,7 @@
       <c r="D53" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="E53" s="43"/>
+      <c r="E53" s="49"/>
       <c r="F53" s="6" t="s">
         <v>367</v>
       </c>

</xml_diff>

<commit_message>
Corrected the names of medium and cattle egrets. Other fixed issues are : fixes #12 closes #13 resolves #14
</commit_message>
<xml_diff>
--- a/uomBirds.xlsx
+++ b/uomBirds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8F854C-0F9F-404A-AD50-E1ED9A3C5E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7880F5F8-5298-4935-A401-08E962BA6ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="521">
   <si>
     <t>Common Name</t>
   </si>
@@ -967,9 +967,6 @@
     <t>ASIAN PALM-SWIFT</t>
   </si>
   <si>
-    <t>Median Egret</t>
-  </si>
-  <si>
     <t>INDIAN POND-HERON</t>
   </si>
   <si>
@@ -979,9 +976,6 @@
     <t>STRIATED HERON</t>
   </si>
   <si>
-    <t>Western Cattle Egret</t>
-  </si>
-  <si>
     <t>Large-billed Crow</t>
   </si>
   <si>
@@ -1565,6 +1559,30 @@
   </si>
   <si>
     <t>Primarily consume fish, occasionally on crustaceans and amphibians. They engage in diving to capture their prey and resurface to swallow it.</t>
+  </si>
+  <si>
+    <t>Eastern Cattle Egret</t>
+  </si>
+  <si>
+    <t>FOREST WAGTAIL</t>
+  </si>
+  <si>
+    <t>Dendronanthus indicus</t>
+  </si>
+  <si>
+    <t>Observed multiple times but only at hotspot 2, Kaju kele.</t>
+  </si>
+  <si>
+    <t>This unique wagtail is easily recognizable due to its specific wing and breast markings. It features a noticeable light-colored stripe above the eye, accompanied by two curved black bands on the upper part of the chest; the lower band being wider if it's there. Its back and wings are a mix of brown and gray with a hint of green, adorned with two distinct white bars across the wings amidst the black plumage.</t>
+  </si>
+  <si>
+    <t>The diet primarily includes tiny invertebrates like ants, beetles, small grasshoppers, butterflies, cicadas, and various other insects. It also includes spiders, small mollusks, and worms.</t>
+  </si>
+  <si>
+    <t>Medium Egret</t>
+  </si>
+  <si>
+    <t>Fairly common winter migrant throughout. Paths and open spaces in wooded areas are the preferred habitat.</t>
   </si>
 </sst>
 </file>
@@ -1730,7 +1748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1796,7 +1814,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2015,11 +2032,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E53" sqref="E53"/>
+      <selection pane="topRight" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2111,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="46" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
@@ -2103,7 +2120,7 @@
         <v>13</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2138,13 +2155,13 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="46" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>16</v>
@@ -2182,16 +2199,16 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="46" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -2226,10 +2243,10 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="46" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>21</v>
@@ -2272,16 +2289,16 @@
         <v>310</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>296</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -2319,10 +2336,10 @@
         <v>247</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I7" s="32" t="s">
         <v>25</v>
@@ -2362,16 +2379,16 @@
         <v>311</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2409,13 +2426,13 @@
         <v>247</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2453,13 +2470,13 @@
         <v>247</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2497,10 +2514,10 @@
         <v>247</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>33</v>
@@ -2544,7 +2561,7 @@
         <v>37</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>38</v>
@@ -2582,16 +2599,16 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="46" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>41</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -2626,16 +2643,16 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="47" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2669,13 +2686,13 @@
         <v>216</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>315</v>
+        <v>519</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>247</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>47</v>
@@ -2719,7 +2736,7 @@
         <v>247</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>51</v>
@@ -2747,7 +2764,7 @@
     </row>
     <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>53</v>
@@ -2763,13 +2780,13 @@
         <v>247</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2791,7 +2808,7 @@
     </row>
     <row r="18" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>55</v>
@@ -2807,7 +2824,7 @@
         <v>247</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>56</v>
@@ -2851,13 +2868,13 @@
         <v>249</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>60</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2879,7 +2896,7 @@
     </row>
     <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>282</v>
@@ -2901,7 +2918,7 @@
         <v>297</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2935,19 +2952,19 @@
         <v>216</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>319</v>
+        <v>513</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>306</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>307</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2988,10 +3005,10 @@
         <v>309</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -3026,16 +3043,16 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="20" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>299</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -3073,10 +3090,10 @@
         <v>250</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>63</v>
@@ -3114,16 +3131,16 @@
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="20" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>292</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -3161,13 +3178,13 @@
         <v>251</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -3205,13 +3222,13 @@
         <v>252</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3249,13 +3266,13 @@
         <v>253</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -3293,7 +3310,7 @@
         <v>75</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>76</v>
@@ -3334,10 +3351,10 @@
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="48" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>80</v>
@@ -3378,7 +3395,7 @@
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="48" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>83</v>
@@ -3422,16 +3439,16 @@
       </c>
       <c r="E32" s="36"/>
       <c r="F32" s="36" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G32" s="36" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H32" s="36" t="s">
         <v>290</v>
       </c>
       <c r="I32" s="36" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -3469,13 +3486,13 @@
         <v>89</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>90</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -3509,19 +3526,19 @@
         <v>216</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F34" s="46" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>93</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -3558,16 +3575,16 @@
         <v>219</v>
       </c>
       <c r="F35" s="46" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>97</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3589,7 +3606,7 @@
     </row>
     <row r="36" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>98</v>
@@ -3601,19 +3618,19 @@
         <v>216</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>99</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -3648,16 +3665,16 @@
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>102</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -3692,7 +3709,7 @@
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>105</v>
@@ -3701,7 +3718,7 @@
         <v>106</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -3736,16 +3753,16 @@
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>109</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
@@ -3780,16 +3797,16 @@
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>291</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -3827,13 +3844,13 @@
         <v>254</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>113</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -3855,7 +3872,7 @@
     </row>
     <row r="42" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>114</v>
@@ -3871,13 +3888,13 @@
         <v>255</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>115</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -3915,13 +3932,13 @@
         <v>248</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>118</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -3959,13 +3976,13 @@
         <v>285</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>289</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -4003,13 +4020,13 @@
         <v>248</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>122</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -4044,16 +4061,16 @@
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>293</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -4075,7 +4092,7 @@
     </row>
     <row r="47" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>220</v>
@@ -4088,7 +4105,7 @@
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>124</v>
@@ -4097,7 +4114,7 @@
         <v>125</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -4132,7 +4149,7 @@
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>127</v>
@@ -4141,7 +4158,7 @@
         <v>128</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -4163,7 +4180,7 @@
     </row>
     <row r="49" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B49" s="22" t="s">
         <v>222</v>
@@ -4175,13 +4192,13 @@
         <v>216</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H49" s="13" t="s">
         <v>129</v>
@@ -4209,7 +4226,7 @@
     </row>
     <row r="50" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>131</v>
@@ -4222,16 +4239,16 @@
       </c>
       <c r="E50" s="43"/>
       <c r="F50" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>133</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -4265,19 +4282,19 @@
         <v>216</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>137</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -4302,7 +4319,7 @@
         <v>138</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>139</v>
@@ -4312,7 +4329,7 @@
       </c>
       <c r="E52" s="43"/>
       <c r="F52" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>140</v>
@@ -4321,7 +4338,7 @@
         <v>141</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -4343,29 +4360,29 @@
     </row>
     <row r="53" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>143</v>
+        <v>514</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>515</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D53" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="E53" s="49"/>
+      <c r="D53" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="E53" s="43"/>
       <c r="F53" s="6" t="s">
-        <v>367</v>
+        <v>516</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>432</v>
+        <v>520</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>144</v>
+        <v>517</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -4387,29 +4404,29 @@
     </row>
     <row r="54" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D54" s="21" t="s">
         <v>216</v>
       </c>
       <c r="E54" s="4"/>
-      <c r="F54" s="26" t="s">
-        <v>368</v>
+      <c r="F54" s="6" t="s">
+        <v>365</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -4430,30 +4447,30 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="B55" s="30" t="s">
-        <v>148</v>
+      <c r="A55" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>145</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D55" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="E55" s="43"/>
-      <c r="F55" s="6" t="s">
-        <v>149</v>
+      <c r="D55" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="26" t="s">
+        <v>366</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>150</v>
+        <v>412</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4473,31 +4490,31 @@
       <c r="Y55" s="4"/>
       <c r="Z55" s="4"/>
     </row>
-    <row r="56" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>224</v>
+    <row r="56" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>148</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D56" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4" t="s">
-        <v>369</v>
+      <c r="D56" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="E56" s="43"/>
+      <c r="F56" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>415</v>
+        <v>150</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -4519,29 +4536,29 @@
     </row>
     <row r="57" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B57" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="C57" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D57" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="E57" s="43"/>
+      <c r="D57" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E57" s="4"/>
       <c r="F57" s="4" t="s">
-        <v>286</v>
+        <v>367</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>300</v>
+        <v>413</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>294</v>
+        <v>152</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4561,31 +4578,31 @@
       <c r="Y57" s="4"/>
       <c r="Z57" s="4"/>
     </row>
-    <row r="58" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="6" t="s">
-        <v>370</v>
+    <row r="58" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B58" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="E58" s="43"/>
+      <c r="F58" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>416</v>
+        <v>300</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>155</v>
+        <v>294</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4607,10 +4624,10 @@
     </row>
     <row r="59" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>331</v>
+        <v>239</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>154</v>
@@ -4618,20 +4635,18 @@
       <c r="D59" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="E59" s="4" t="s">
-        <v>332</v>
-      </c>
+      <c r="E59" s="4"/>
       <c r="F59" s="6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -4652,27 +4667,29 @@
       <c r="Z59" s="4"/>
     </row>
     <row r="60" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>159</v>
+      <c r="A60" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D60" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="E60" s="43"/>
+        <v>154</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>330</v>
+      </c>
       <c r="F60" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>161</v>
+        <v>421</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>494</v>
@@ -4696,30 +4713,30 @@
       <c r="Z60" s="4"/>
     </row>
     <row r="61" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>163</v>
+      <c r="A61" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D61" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="E61" s="4"/>
+      <c r="D61" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="E61" s="43"/>
       <c r="F61" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>417</v>
+        <v>161</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I61" s="32" t="s">
-        <v>493</v>
+        <v>162</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>492</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -4739,31 +4756,31 @@
       <c r="Y61" s="4"/>
       <c r="Z61" s="4"/>
     </row>
-    <row r="62" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>165</v>
+    <row r="62" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D62" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D62" s="21" t="s">
         <v>216</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="6" t="s">
-        <v>249</v>
+        <v>371</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>495</v>
+        <v>164</v>
+      </c>
+      <c r="I62" s="32" t="s">
+        <v>491</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -4785,29 +4802,29 @@
     </row>
     <row r="63" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>170</v>
+        <v>241</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>216</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="6" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>172</v>
+        <v>493</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -4828,30 +4845,30 @@
       <c r="Z63" s="4"/>
     </row>
     <row r="64" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A64" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="B64" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="C64" s="32" t="s">
+      <c r="A64" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>169</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="6" t="s">
         <v>247</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -4872,30 +4889,30 @@
       <c r="Z64" s="4"/>
     </row>
     <row r="65" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>177</v>
+      <c r="A65" s="41" t="s">
+        <v>173</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C65" s="32" t="s">
         <v>169</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="E65" s="4"/>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="6" t="s">
         <v>247</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>514</v>
+        <v>176</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -4915,31 +4932,31 @@
       <c r="Y65" s="4"/>
       <c r="Z65" s="4"/>
     </row>
-    <row r="66" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="C66" s="38" t="s">
-        <v>181</v>
+    <row r="66" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>169</v>
       </c>
       <c r="D66" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E66" s="13"/>
-      <c r="F66" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="G66" s="13" t="s">
-        <v>422</v>
-      </c>
-      <c r="H66" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="I66" s="13" t="s">
-        <v>497</v>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>512</v>
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
@@ -4960,30 +4977,30 @@
       <c r="Z66" s="4"/>
     </row>
     <row r="67" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="40" t="s">
-        <v>334</v>
+      <c r="A67" s="7" t="s">
+        <v>331</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>226</v>
+        <v>181</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>216</v>
       </c>
       <c r="E67" s="13"/>
       <c r="F67" s="6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I67" s="13" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
@@ -5004,30 +5021,30 @@
       <c r="Z67" s="4"/>
     </row>
     <row r="68" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>242</v>
+      <c r="A68" s="40" t="s">
+        <v>332</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C68" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="C68" s="38" t="s">
         <v>226</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E68" s="4"/>
+      <c r="E68" s="13"/>
       <c r="F68" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>499</v>
+        <v>374</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>496</v>
       </c>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
@@ -5049,29 +5066,29 @@
     </row>
     <row r="69" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>216</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="6" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>189</v>
+        <v>433</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
@@ -5091,12 +5108,12 @@
       <c r="Y69" s="4"/>
       <c r="Z69" s="4"/>
     </row>
-    <row r="70" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>191</v>
+    <row r="70" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>187</v>
       </c>
       <c r="C70" s="32" t="s">
         <v>188</v>
@@ -5105,17 +5122,17 @@
         <v>216</v>
       </c>
       <c r="E70" s="4"/>
-      <c r="F70" s="4" t="s">
-        <v>378</v>
+      <c r="F70" s="6" t="s">
+        <v>371</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>436</v>
+        <v>189</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
@@ -5135,31 +5152,31 @@
       <c r="Y70" s="4"/>
       <c r="Z70" s="4"/>
     </row>
-    <row r="71" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B71" s="18" t="s">
-        <v>193</v>
+    <row r="71" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>191</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D71" s="15" t="s">
         <v>216</v>
       </c>
       <c r="E71" s="4"/>
-      <c r="F71" s="6" t="s">
-        <v>256</v>
+      <c r="F71" s="4" t="s">
+        <v>376</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>196</v>
+        <v>434</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>198</v>
+        <v>499</v>
       </c>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
@@ -5180,11 +5197,11 @@
       <c r="Z71" s="4"/>
     </row>
     <row r="72" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="44" t="s">
-        <v>336</v>
+      <c r="A72" s="5" t="s">
+        <v>245</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="C72" s="32" t="s">
         <v>194</v>
@@ -5192,20 +5209,18 @@
       <c r="D72" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E72" s="5" t="s">
-        <v>335</v>
-      </c>
+      <c r="E72" s="4"/>
       <c r="F72" s="6" t="s">
-        <v>195</v>
+        <v>256</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>502</v>
+        <v>198</v>
       </c>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
@@ -5225,31 +5240,33 @@
       <c r="Y72" s="4"/>
       <c r="Z72" s="4"/>
     </row>
-    <row r="73" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B73" s="27" t="s">
-        <v>283</v>
-      </c>
-      <c r="C73" t="s">
-        <v>284</v>
+    <row r="73" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>194</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4" t="s">
-        <v>287</v>
+      <c r="E73" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>437</v>
+        <v>199</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>298</v>
+        <v>200</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
@@ -5269,33 +5286,31 @@
       <c r="Y73" s="4"/>
       <c r="Z73" s="4"/>
     </row>
-    <row r="74" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A74" s="44" t="s">
-        <v>339</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="C74" s="32" t="s">
-        <v>202</v>
+    <row r="74" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B74" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C74" t="s">
+        <v>284</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="E74" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>379</v>
+        <v>216</v>
+      </c>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4" t="s">
+        <v>287</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>203</v>
+        <v>298</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
@@ -5317,31 +5332,31 @@
     </row>
     <row r="75" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" s="44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C75" s="32" t="s">
         <v>202</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
@@ -5362,27 +5377,29 @@
       <c r="Z75" s="4"/>
     </row>
     <row r="76" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B76" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>208</v>
+      <c r="A76" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>202</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E76" s="4"/>
+      <c r="E76" s="20" t="s">
+        <v>338</v>
+      </c>
       <c r="F76" s="6" t="s">
-        <v>352</v>
+        <v>378</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>209</v>
+        <v>437</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>505</v>
@@ -5407,29 +5424,29 @@
     </row>
     <row r="77" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>216</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="6" t="s">
-        <v>247</v>
+        <v>350</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>440</v>
+        <v>209</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>214</v>
+        <v>503</v>
       </c>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
@@ -5449,33 +5466,31 @@
       <c r="Y77" s="4"/>
       <c r="Z77" s="4"/>
     </row>
-    <row r="78" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="B78" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="C78" s="31" t="s">
-        <v>279</v>
+    <row r="78" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="D78" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E78" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>381</v>
+      <c r="E78" s="4"/>
+      <c r="F78" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>295</v>
+        <v>213</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>506</v>
+        <v>214</v>
       </c>
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
@@ -5496,15 +5511,33 @@
       <c r="Z78" s="4"/>
     </row>
     <row r="79" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
+      <c r="A79" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B79" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C79" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>504</v>
+      </c>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
@@ -31255,10 +31288,38 @@
       <c r="Y998" s="4"/>
       <c r="Z998" s="4"/>
     </row>
+    <row r="999" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A999" s="4"/>
+      <c r="B999" s="4"/>
+      <c r="C999" s="4"/>
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+      <c r="G999" s="4"/>
+      <c r="H999" s="4"/>
+      <c r="I999" s="4"/>
+      <c r="J999" s="4"/>
+      <c r="K999" s="4"/>
+      <c r="L999" s="4"/>
+      <c r="M999" s="4"/>
+      <c r="N999" s="4"/>
+      <c r="O999" s="4"/>
+      <c r="P999" s="4"/>
+      <c r="Q999" s="4"/>
+      <c r="R999" s="4"/>
+      <c r="S999" s="4"/>
+      <c r="T999" s="4"/>
+      <c r="U999" s="4"/>
+      <c r="V999" s="4"/>
+      <c r="W999" s="4"/>
+      <c r="X999" s="4"/>
+      <c r="Y999" s="4"/>
+      <c r="Z999" s="4"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I998">
-    <sortCondition ref="C1:C998"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I999">
+    <sortCondition ref="C1:C999"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>